<commit_message>
reviews and updates by Ragab
</commit_message>
<xml_diff>
--- a/Lhub_RTM_v1.xlsx
+++ b/Lhub_RTM_v1.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Farah\Desktop\V1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI subjects\software project management\project 3\Learning-hub\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7752"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
   <si>
     <t>Requirements Traceability Matrix</t>
   </si>
@@ -87,9 +87,6 @@
     <t>SIQ_7</t>
   </si>
   <si>
-    <t>SIQ_3</t>
-  </si>
-  <si>
     <t>SIQ_11</t>
   </si>
   <si>
@@ -168,9 +165,6 @@
     <t>Lhub_SRS_2.4.1.5</t>
   </si>
   <si>
-    <t>Lhub_SRS_2.4.1.6</t>
-  </si>
-  <si>
     <t>Lhub_SRS_2.4.2.1</t>
   </si>
   <si>
@@ -198,15 +192,6 @@
     <t>Lhub_SRS_2.4.3.6</t>
   </si>
   <si>
-    <t>Lhub_SRS_2.4.3.7</t>
-  </si>
-  <si>
-    <t>Lhub_SRS_2.4.3.8</t>
-  </si>
-  <si>
-    <t>Lhub_SRS_2.4.3.9</t>
-  </si>
-  <si>
     <t>Lhub_SRS_2.4.4.2</t>
   </si>
   <si>
@@ -225,9 +210,6 @@
     <t>SIQ_35</t>
   </si>
   <si>
-    <t>SIQ_23</t>
-  </si>
-  <si>
     <t>SIQ_29</t>
   </si>
   <si>
@@ -247,6 +229,15 @@
   </si>
   <si>
     <t>1.0</t>
+  </si>
+  <si>
+    <t>SIQ_22</t>
+  </si>
+  <si>
+    <t>Changes in SRS IDs and SIQ IDs</t>
+  </si>
+  <si>
+    <t>Ragab</t>
   </si>
 </sst>
 </file>
@@ -577,7 +568,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -624,9 +615,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -657,12 +645,69 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="15" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -672,13 +717,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -705,54 +744,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="15" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -1078,23 +1078,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z32"/>
+  <dimension ref="A1:Z34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" style="16" customWidth="1"/>
-    <col min="2" max="2" width="30.42578125" style="16" customWidth="1"/>
-    <col min="3" max="3" width="48.140625" style="16" customWidth="1"/>
-    <col min="4" max="4" width="23.28515625" style="16" customWidth="1"/>
-    <col min="5" max="5" width="35.85546875" style="16" customWidth="1"/>
+    <col min="1" max="1" width="23.33203125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="30.44140625" style="16" customWidth="1"/>
+    <col min="3" max="3" width="48.109375" style="16" customWidth="1"/>
+    <col min="4" max="4" width="23.33203125" style="16" customWidth="1"/>
+    <col min="5" max="5" width="35.88671875" style="16" customWidth="1"/>
     <col min="6" max="6" width="38" style="16" customWidth="1"/>
-    <col min="7" max="7" width="37.5703125" style="16" customWidth="1"/>
-    <col min="8" max="8" width="44.5703125" style="16" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="16"/>
+    <col min="7" max="7" width="37.5546875" style="16" customWidth="1"/>
+    <col min="8" max="8" width="44.5546875" style="16" customWidth="1"/>
+    <col min="9" max="16384" width="9.109375" style="16"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1">
@@ -1103,62 +1103,66 @@
       </c>
     </row>
     <row r="2" spans="1:26" s="5" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A2" s="60" t="s">
+      <c r="A2" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="58"/>
-      <c r="D2" s="49" t="s">
-        <v>67</v>
-      </c>
-      <c r="E2" s="50" t="s">
+      <c r="C2" s="46"/>
+      <c r="D2" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="F2" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="G2" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="H2" s="32" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" s="5" customFormat="1" ht="23.25" customHeight="1">
+      <c r="A3" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="46"/>
+      <c r="D3" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" s="29">
+        <v>43588</v>
+      </c>
+      <c r="F3" s="29">
+        <v>43529</v>
+      </c>
+      <c r="G3" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="F2" s="50" t="s">
+      <c r="H3" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="G2" s="50" t="s">
-        <v>70</v>
-      </c>
-      <c r="H2" s="51" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" s="5" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A3" s="60" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="58" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="58"/>
-      <c r="D3" s="52" t="s">
-        <v>72</v>
-      </c>
-      <c r="E3" s="48">
-        <v>43587</v>
-      </c>
-      <c r="F3" s="48">
-        <v>43501</v>
-      </c>
-      <c r="G3" s="53"/>
-      <c r="H3" s="54"/>
     </row>
     <row r="4" spans="1:26" s="5" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
-      <c r="A4" s="60" t="s">
+      <c r="A4" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="59">
+      <c r="B4" s="47">
         <v>43470</v>
       </c>
-      <c r="C4" s="59"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="56"/>
-      <c r="F4" s="56"/>
-      <c r="G4" s="56"/>
-      <c r="H4" s="57"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="38"/>
     </row>
     <row r="5" spans="1:26" s="7" customFormat="1" ht="33.75" customHeight="1">
       <c r="A5" s="1" t="s">
@@ -1205,22 +1209,22 @@
       <c r="Z5" s="6"/>
     </row>
     <row r="6" spans="1:26" s="9" customFormat="1" ht="24.75" customHeight="1">
-      <c r="A6" s="46">
+      <c r="A6" s="40">
         <v>1</v>
       </c>
-      <c r="B6" s="45" t="s">
-        <v>33</v>
+      <c r="B6" s="48" t="s">
+        <v>32</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="47"/>
+      <c r="D6" s="41"/>
       <c r="E6" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" s="29"/>
-      <c r="G6" s="29"/>
-      <c r="H6" s="29"/>
+        <v>30</v>
+      </c>
+      <c r="F6" s="42"/>
+      <c r="G6" s="42"/>
+      <c r="H6" s="42"/>
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
       <c r="K6" s="8"/>
@@ -1241,18 +1245,18 @@
       <c r="Z6" s="8"/>
     </row>
     <row r="7" spans="1:26" s="9" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A7" s="46"/>
-      <c r="B7" s="45"/>
+      <c r="A7" s="40"/>
+      <c r="B7" s="48"/>
       <c r="C7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="47"/>
+      <c r="D7" s="41"/>
       <c r="E7" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="30"/>
+        <v>31</v>
+      </c>
+      <c r="F7" s="43"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
       <c r="K7" s="8"/>
@@ -1273,22 +1277,22 @@
       <c r="Z7" s="8"/>
     </row>
     <row r="8" spans="1:26" s="9" customFormat="1" ht="18" customHeight="1">
-      <c r="A8" s="34">
+      <c r="A8" s="44">
         <v>2</v>
       </c>
-      <c r="B8" s="31" t="s">
-        <v>34</v>
+      <c r="B8" s="49" t="s">
+        <v>33</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="37"/>
+      <c r="D8" s="53"/>
       <c r="E8" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F8" s="40"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
+        <v>40</v>
+      </c>
+      <c r="F8" s="56"/>
+      <c r="G8" s="44"/>
+      <c r="H8" s="44"/>
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
       <c r="K8" s="8"/>
@@ -1309,18 +1313,18 @@
       <c r="Z8" s="8"/>
     </row>
     <row r="9" spans="1:26" s="9" customFormat="1" ht="21" customHeight="1">
-      <c r="A9" s="35"/>
-      <c r="B9" s="32"/>
+      <c r="A9" s="52"/>
+      <c r="B9" s="50"/>
       <c r="C9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="38"/>
+      <c r="D9" s="54"/>
       <c r="E9" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="F9" s="41"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="36"/>
+        <v>41</v>
+      </c>
+      <c r="F9" s="57"/>
+      <c r="G9" s="45"/>
+      <c r="H9" s="45"/>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
@@ -1341,16 +1345,16 @@
       <c r="Z9" s="8"/>
     </row>
     <row r="10" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A10" s="35"/>
-      <c r="B10" s="32"/>
-      <c r="C10" s="25" t="s">
+      <c r="A10" s="52"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="38"/>
+      <c r="D10" s="54"/>
       <c r="E10" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="F10" s="41"/>
+        <v>42</v>
+      </c>
+      <c r="F10" s="57"/>
       <c r="G10" s="10"/>
       <c r="H10" s="15"/>
       <c r="I10" s="8"/>
@@ -1373,16 +1377,16 @@
       <c r="Z10" s="8"/>
     </row>
     <row r="11" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A11" s="35"/>
-      <c r="B11" s="32"/>
-      <c r="C11" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="D11" s="38"/>
+      <c r="A11" s="52"/>
+      <c r="B11" s="50"/>
+      <c r="C11" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="54"/>
       <c r="E11" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="F11" s="41"/>
+        <v>43</v>
+      </c>
+      <c r="F11" s="57"/>
       <c r="G11" s="10"/>
       <c r="H11" s="15"/>
       <c r="I11" s="8"/>
@@ -1405,14 +1409,14 @@
       <c r="Z11" s="8"/>
     </row>
     <row r="12" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A12" s="35"/>
-      <c r="B12" s="32"/>
-      <c r="C12" s="43"/>
-      <c r="D12" s="38"/>
+      <c r="A12" s="52"/>
+      <c r="B12" s="50"/>
+      <c r="C12" s="59"/>
+      <c r="D12" s="54"/>
       <c r="E12" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="F12" s="41"/>
+        <v>44</v>
+      </c>
+      <c r="F12" s="57"/>
       <c r="G12" s="10"/>
       <c r="H12" s="15"/>
       <c r="I12" s="8"/>
@@ -1435,14 +1439,14 @@
       <c r="Z12" s="8"/>
     </row>
     <row r="13" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A13" s="35"/>
-      <c r="B13" s="32"/>
-      <c r="C13" s="43"/>
-      <c r="D13" s="38"/>
+      <c r="A13" s="52"/>
+      <c r="B13" s="50"/>
+      <c r="C13" s="59"/>
+      <c r="D13" s="54"/>
       <c r="E13" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="F13" s="41"/>
+        <v>45</v>
+      </c>
+      <c r="F13" s="57"/>
       <c r="G13" s="10"/>
       <c r="H13" s="15"/>
       <c r="I13" s="8"/>
@@ -1465,14 +1469,14 @@
       <c r="Z13" s="8"/>
     </row>
     <row r="14" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A14" s="35"/>
-      <c r="B14" s="32"/>
-      <c r="C14" s="43"/>
-      <c r="D14" s="38"/>
+      <c r="A14" s="52"/>
+      <c r="B14" s="50"/>
+      <c r="C14" s="59"/>
+      <c r="D14" s="54"/>
       <c r="E14" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="F14" s="41"/>
+        <v>46</v>
+      </c>
+      <c r="F14" s="57"/>
       <c r="G14" s="10"/>
       <c r="H14" s="15"/>
       <c r="I14" s="8"/>
@@ -1495,14 +1499,14 @@
       <c r="Z14" s="8"/>
     </row>
     <row r="15" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A15" s="35"/>
-      <c r="B15" s="32"/>
-      <c r="C15" s="43"/>
-      <c r="D15" s="38"/>
+      <c r="A15" s="45"/>
+      <c r="B15" s="51"/>
+      <c r="C15" s="60"/>
+      <c r="D15" s="55"/>
       <c r="E15" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="F15" s="41"/>
+        <v>47</v>
+      </c>
+      <c r="F15" s="58"/>
       <c r="G15" s="10"/>
       <c r="H15" s="15"/>
       <c r="I15" s="8"/>
@@ -1524,15 +1528,20 @@
       <c r="Y15" s="8"/>
       <c r="Z15" s="8"/>
     </row>
-    <row r="16" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A16" s="36"/>
-      <c r="B16" s="33"/>
-      <c r="C16" s="44"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="F16" s="42"/>
+    <row r="16" spans="1:26" s="9" customFormat="1" ht="27" customHeight="1">
+      <c r="A16" s="44">
+        <v>3</v>
+      </c>
+      <c r="B16" s="49" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="F16" s="14"/>
       <c r="G16" s="10"/>
       <c r="H16" s="15"/>
       <c r="I16" s="8"/>
@@ -1555,21 +1564,14 @@
       <c r="Z16" s="8"/>
     </row>
     <row r="17" spans="1:26" s="9" customFormat="1" ht="27" customHeight="1">
-      <c r="A17" s="10">
-        <v>3</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>35</v>
-      </c>
+      <c r="A17" s="52"/>
+      <c r="B17" s="50"/>
       <c r="C17" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D17" s="12"/>
-      <c r="E17" s="28" t="s">
-        <v>50</v>
-      </c>
-      <c r="F17" s="14"/>
-      <c r="G17" s="10"/>
+        <v>20</v>
+      </c>
+      <c r="E17" s="27"/>
+      <c r="F17" s="61"/>
+      <c r="G17" s="28"/>
       <c r="H17" s="15"/>
       <c r="I17" s="8"/>
       <c r="J17" s="8"/>
@@ -1590,22 +1592,15 @@
       <c r="Y17" s="8"/>
       <c r="Z17" s="8"/>
     </row>
-    <row r="18" spans="1:26" s="9" customFormat="1" ht="21.75" customHeight="1">
-      <c r="A18" s="34">
-        <v>4</v>
-      </c>
-      <c r="B18" s="31" t="s">
-        <v>36</v>
-      </c>
+    <row r="18" spans="1:26" s="9" customFormat="1" ht="27" customHeight="1">
+      <c r="A18" s="52"/>
+      <c r="B18" s="50"/>
       <c r="C18" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D18" s="37"/>
-      <c r="E18" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="F18" s="19"/>
-      <c r="G18" s="22"/>
+        <v>21</v>
+      </c>
+      <c r="E18" s="27"/>
+      <c r="F18" s="61"/>
+      <c r="G18" s="28"/>
       <c r="H18" s="15"/>
       <c r="I18" s="8"/>
       <c r="J18" s="8"/>
@@ -1626,18 +1621,16 @@
       <c r="Y18" s="8"/>
       <c r="Z18" s="8"/>
     </row>
-    <row r="19" spans="1:26" s="9" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A19" s="35"/>
-      <c r="B19" s="32"/>
+    <row r="19" spans="1:26" s="9" customFormat="1" ht="27" customHeight="1">
+      <c r="A19" s="52"/>
+      <c r="B19" s="50"/>
       <c r="C19" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D19" s="38"/>
-      <c r="E19" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="F19" s="20"/>
-      <c r="G19" s="23"/>
+        <v>22</v>
+      </c>
+      <c r="D19" s="24"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="61"/>
+      <c r="G19" s="28"/>
       <c r="H19" s="15"/>
       <c r="I19" s="8"/>
       <c r="J19" s="8"/>
@@ -1658,18 +1651,16 @@
       <c r="Y19" s="8"/>
       <c r="Z19" s="8"/>
     </row>
-    <row r="20" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A20" s="35"/>
-      <c r="B20" s="32"/>
+    <row r="20" spans="1:26" s="9" customFormat="1" ht="27" customHeight="1">
+      <c r="A20" s="45"/>
+      <c r="B20" s="51"/>
       <c r="C20" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D20" s="38"/>
-      <c r="E20" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="F20" s="20"/>
-      <c r="G20" s="23"/>
+        <v>23</v>
+      </c>
+      <c r="D20" s="24"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="61"/>
+      <c r="G20" s="28"/>
       <c r="H20" s="15"/>
       <c r="I20" s="8"/>
       <c r="J20" s="8"/>
@@ -1690,16 +1681,22 @@
       <c r="Y20" s="8"/>
       <c r="Z20" s="8"/>
     </row>
-    <row r="21" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A21" s="35"/>
-      <c r="B21" s="32"/>
+    <row r="21" spans="1:26" s="9" customFormat="1" ht="21.75" customHeight="1">
+      <c r="A21" s="44">
+        <v>4</v>
+      </c>
+      <c r="B21" s="49" t="s">
+        <v>35</v>
+      </c>
       <c r="C21" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D21" s="38"/>
-      <c r="E21" s="29"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="23"/>
+        <v>24</v>
+      </c>
+      <c r="D21" s="53"/>
+      <c r="E21" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="F21" s="18"/>
+      <c r="G21" s="21"/>
       <c r="H21" s="15"/>
       <c r="I21" s="8"/>
       <c r="J21" s="8"/>
@@ -1720,16 +1717,18 @@
       <c r="Y21" s="8"/>
       <c r="Z21" s="8"/>
     </row>
-    <row r="22" spans="1:26" s="9" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A22" s="36"/>
-      <c r="B22" s="33"/>
+    <row r="22" spans="1:26" s="9" customFormat="1" ht="23.25" customHeight="1">
+      <c r="A22" s="52"/>
+      <c r="B22" s="50"/>
       <c r="C22" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D22" s="39"/>
-      <c r="E22" s="30"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="24"/>
+        <v>25</v>
+      </c>
+      <c r="D22" s="54"/>
+      <c r="E22" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="F22" s="19"/>
+      <c r="G22" s="22"/>
       <c r="H22" s="15"/>
       <c r="I22" s="8"/>
       <c r="J22" s="8"/>
@@ -1750,22 +1749,16 @@
       <c r="Y22" s="8"/>
       <c r="Z22" s="8"/>
     </row>
-    <row r="23" spans="1:26" s="9" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A23" s="34">
-        <v>5</v>
-      </c>
-      <c r="B23" s="31" t="s">
-        <v>37</v>
-      </c>
+    <row r="23" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A23" s="52"/>
+      <c r="B23" s="50"/>
       <c r="C23" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D23" s="37"/>
-      <c r="E23" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="F23" s="14"/>
-      <c r="G23" s="10"/>
+        <v>26</v>
+      </c>
+      <c r="D23" s="54"/>
+      <c r="E23" s="63"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="22"/>
       <c r="H23" s="15"/>
       <c r="I23" s="8"/>
       <c r="J23" s="8"/>
@@ -1786,18 +1779,14 @@
       <c r="Y23" s="8"/>
       <c r="Z23" s="8"/>
     </row>
-    <row r="24" spans="1:26" s="9" customFormat="1" ht="21" customHeight="1">
-      <c r="A24" s="35"/>
-      <c r="B24" s="32"/>
-      <c r="C24" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D24" s="38"/>
-      <c r="E24" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="F24" s="14"/>
-      <c r="G24" s="10"/>
+    <row r="24" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A24" s="52"/>
+      <c r="B24" s="50"/>
+      <c r="C24" s="62"/>
+      <c r="D24" s="54"/>
+      <c r="E24" s="64"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="22"/>
       <c r="H24" s="15"/>
       <c r="I24" s="8"/>
       <c r="J24" s="8"/>
@@ -1818,18 +1807,14 @@
       <c r="Y24" s="8"/>
       <c r="Z24" s="8"/>
     </row>
-    <row r="25" spans="1:26" s="9" customFormat="1" ht="21" customHeight="1">
-      <c r="A25" s="36"/>
-      <c r="B25" s="33"/>
-      <c r="C25" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D25" s="39"/>
-      <c r="E25" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="F25" s="14"/>
-      <c r="G25" s="10"/>
+    <row r="25" spans="1:26" s="9" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A25" s="45"/>
+      <c r="B25" s="51"/>
+      <c r="C25" s="60"/>
+      <c r="D25" s="55"/>
+      <c r="E25" s="65"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="23"/>
       <c r="H25" s="15"/>
       <c r="I25" s="8"/>
       <c r="J25" s="8"/>
@@ -1850,19 +1835,18 @@
       <c r="Y25" s="8"/>
       <c r="Z25" s="8"/>
     </row>
-    <row r="26" spans="1:26" s="9" customFormat="1" ht="21" customHeight="1">
-      <c r="A26" s="34">
-        <v>6</v>
-      </c>
-      <c r="B26" s="31" t="s">
-        <v>38</v>
+    <row r="26" spans="1:26" s="9" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A26" s="44">
+        <v>5</v>
+      </c>
+      <c r="B26" s="49" t="s">
+        <v>36</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D26" s="37"/>
+        <v>27</v>
+      </c>
       <c r="E26" s="13" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="F26" s="14"/>
       <c r="G26" s="10"/>
@@ -1886,16 +1870,13 @@
       <c r="Y26" s="8"/>
       <c r="Z26" s="8"/>
     </row>
-    <row r="27" spans="1:26" s="9" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A27" s="35"/>
-      <c r="B27" s="32"/>
+    <row r="27" spans="1:26" s="9" customFormat="1" ht="21" customHeight="1">
+      <c r="A27" s="52"/>
+      <c r="B27" s="50"/>
       <c r="C27" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D27" s="38"/>
-      <c r="E27" s="13" t="s">
-        <v>58</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="E27" s="13"/>
       <c r="F27" s="14"/>
       <c r="G27" s="10"/>
       <c r="H27" s="15"/>
@@ -1919,15 +1900,12 @@
       <c r="Z27" s="8"/>
     </row>
     <row r="28" spans="1:26" s="9" customFormat="1" ht="21" customHeight="1">
-      <c r="A28" s="35"/>
-      <c r="B28" s="32"/>
+      <c r="A28" s="45"/>
+      <c r="B28" s="51"/>
       <c r="C28" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D28" s="38"/>
-      <c r="E28" s="13" t="s">
-        <v>59</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="E28" s="13"/>
       <c r="F28" s="14"/>
       <c r="G28" s="10"/>
       <c r="H28" s="15"/>
@@ -1951,13 +1929,19 @@
       <c r="Z28" s="8"/>
     </row>
     <row r="29" spans="1:26" s="9" customFormat="1" ht="21" customHeight="1">
-      <c r="A29" s="36"/>
-      <c r="B29" s="33"/>
+      <c r="A29" s="44">
+        <v>6</v>
+      </c>
+      <c r="B29" s="49" t="s">
+        <v>37</v>
+      </c>
       <c r="C29" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D29" s="39"/>
-      <c r="E29" s="18"/>
+        <v>67</v>
+      </c>
+      <c r="D29" s="53"/>
+      <c r="E29" s="13" t="s">
+        <v>52</v>
+      </c>
       <c r="F29" s="14"/>
       <c r="G29" s="10"/>
       <c r="H29" s="15"/>
@@ -1980,17 +1964,13 @@
       <c r="Y29" s="8"/>
       <c r="Z29" s="8"/>
     </row>
-    <row r="30" spans="1:26" s="9" customFormat="1" ht="33" customHeight="1">
-      <c r="A30" s="10">
-        <v>7</v>
-      </c>
-      <c r="B30" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="C30" s="3"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="26" t="s">
-        <v>60</v>
+    <row r="30" spans="1:26" s="9" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A30" s="52"/>
+      <c r="B30" s="50"/>
+      <c r="C30" s="62"/>
+      <c r="D30" s="54"/>
+      <c r="E30" s="13" t="s">
+        <v>53</v>
       </c>
       <c r="F30" s="14"/>
       <c r="G30" s="10"/>
@@ -2014,19 +1994,13 @@
       <c r="Y30" s="8"/>
       <c r="Z30" s="8"/>
     </row>
-    <row r="31" spans="1:26" s="9" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A31" s="10">
-        <v>8</v>
-      </c>
-      <c r="B31" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D31" s="12"/>
-      <c r="E31" s="27" t="s">
-        <v>61</v>
+    <row r="31" spans="1:26" s="9" customFormat="1" ht="21" customHeight="1">
+      <c r="A31" s="52"/>
+      <c r="B31" s="50"/>
+      <c r="C31" s="59"/>
+      <c r="D31" s="54"/>
+      <c r="E31" s="13" t="s">
+        <v>54</v>
       </c>
       <c r="F31" s="14"/>
       <c r="G31" s="10"/>
@@ -2050,17 +2024,17 @@
       <c r="Y31" s="8"/>
       <c r="Z31" s="8"/>
     </row>
-    <row r="32" spans="1:26" s="9" customFormat="1" ht="33.75" customHeight="1">
+    <row r="32" spans="1:26" s="9" customFormat="1" ht="33" customHeight="1">
       <c r="A32" s="10">
-        <v>9</v>
-      </c>
-      <c r="B32" s="26" t="s">
-        <v>62</v>
+        <v>7</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>38</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="12"/>
-      <c r="E32" s="28" t="s">
-        <v>63</v>
+      <c r="E32" s="25" t="s">
+        <v>55</v>
       </c>
       <c r="F32" s="14"/>
       <c r="G32" s="10"/>
@@ -2084,34 +2058,107 @@
       <c r="Y32" s="8"/>
       <c r="Z32" s="8"/>
     </row>
+    <row r="33" spans="1:26" s="9" customFormat="1" ht="33.75" customHeight="1">
+      <c r="A33" s="10">
+        <v>8</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D33" s="12"/>
+      <c r="E33" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="F33" s="14"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="15"/>
+      <c r="I33" s="8"/>
+      <c r="J33" s="8"/>
+      <c r="K33" s="8"/>
+      <c r="L33" s="8"/>
+      <c r="M33" s="8"/>
+      <c r="N33" s="8"/>
+      <c r="O33" s="8"/>
+      <c r="P33" s="8"/>
+      <c r="Q33" s="8"/>
+      <c r="R33" s="8"/>
+      <c r="S33" s="8"/>
+      <c r="T33" s="8"/>
+      <c r="U33" s="8"/>
+      <c r="V33" s="8"/>
+      <c r="W33" s="8"/>
+      <c r="X33" s="8"/>
+      <c r="Y33" s="8"/>
+      <c r="Z33" s="8"/>
+    </row>
+    <row r="34" spans="1:26" s="9" customFormat="1" ht="33.75" customHeight="1">
+      <c r="A34" s="10">
+        <v>9</v>
+      </c>
+      <c r="B34" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="C34" s="3"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="F34" s="14"/>
+      <c r="G34" s="10"/>
+      <c r="H34" s="15"/>
+      <c r="I34" s="8"/>
+      <c r="J34" s="8"/>
+      <c r="K34" s="8"/>
+      <c r="L34" s="8"/>
+      <c r="M34" s="8"/>
+      <c r="N34" s="8"/>
+      <c r="O34" s="8"/>
+      <c r="P34" s="8"/>
+      <c r="Q34" s="8"/>
+      <c r="R34" s="8"/>
+      <c r="S34" s="8"/>
+      <c r="T34" s="8"/>
+      <c r="U34" s="8"/>
+      <c r="V34" s="8"/>
+      <c r="W34" s="8"/>
+      <c r="X34" s="8"/>
+      <c r="Y34" s="8"/>
+      <c r="Z34" s="8"/>
+    </row>
   </sheetData>
-  <mergeCells count="26">
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="H6:H7"/>
+  <mergeCells count="29">
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="D29:D31"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="A8:A15"/>
+    <mergeCell ref="D8:D15"/>
+    <mergeCell ref="F8:F15"/>
+    <mergeCell ref="C12:C15"/>
+    <mergeCell ref="A21:A25"/>
+    <mergeCell ref="B21:B25"/>
+    <mergeCell ref="D21:D25"/>
+    <mergeCell ref="B16:B20"/>
+    <mergeCell ref="A16:A20"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="E23:E25"/>
     <mergeCell ref="G8:G9"/>
     <mergeCell ref="H8:H9"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B8:B16"/>
-    <mergeCell ref="A8:A16"/>
-    <mergeCell ref="D8:D16"/>
-    <mergeCell ref="F8:F16"/>
-    <mergeCell ref="C12:C16"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="D26:D29"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="D23:D25"/>
-    <mergeCell ref="A18:A22"/>
-    <mergeCell ref="B18:B22"/>
-    <mergeCell ref="D18:D22"/>
+    <mergeCell ref="B8:B15"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="H6:H7"/>
   </mergeCells>
   <conditionalFormatting sqref="B5">
     <cfRule type="cellIs" dxfId="5" priority="4" stopIfTrue="1" operator="equal">

</xml_diff>

<commit_message>
added design document and changed SRS IDs
</commit_message>
<xml_diff>
--- a/Lhub_RTM_v1.xlsx
+++ b/Lhub_RTM_v1.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI subjects\software project management\project 3\Learning-hub\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\Project management\Learning-hub project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7752"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="101">
   <si>
     <t>Requirements Traceability Matrix</t>
   </si>
@@ -238,13 +238,106 @@
   </si>
   <si>
     <t>Ragab</t>
+  </si>
+  <si>
+    <t>Lhub_SDD_4.1.2</t>
+  </si>
+  <si>
+    <t>Lhub_SDD_4.1.4</t>
+  </si>
+  <si>
+    <t>Lhub_SDD_4.1.3</t>
+  </si>
+  <si>
+    <t>Lhub_SDD_4.1.1</t>
+  </si>
+  <si>
+    <t>Lhub_SRS_2.4.1.6</t>
+  </si>
+  <si>
+    <t>Lhub_SRS_2.4.1.7</t>
+  </si>
+  <si>
+    <t>Lhub_SRS_2.4.1.8</t>
+  </si>
+  <si>
+    <t>Lhub_SRS_2.4.1.9</t>
+  </si>
+  <si>
+    <t>Lhub_SRS_2.4.1.10</t>
+  </si>
+  <si>
+    <t>Lhub_SRS_2.4.1.11</t>
+  </si>
+  <si>
+    <t>Lhub_SRS_2.4.1.12</t>
+  </si>
+  <si>
+    <t>Lhub_SRS_2.4.1.13</t>
+  </si>
+  <si>
+    <t>Lhub_SRS_2.4.1.14</t>
+  </si>
+  <si>
+    <t>Lhub_SRS_2.4.2.4</t>
+  </si>
+  <si>
+    <t>Lhub_SRS_2.4.2.5</t>
+  </si>
+  <si>
+    <t>Lhub_SRS_2.4.2.6</t>
+  </si>
+  <si>
+    <t>Lhub_SRS_2.4.2.7</t>
+  </si>
+  <si>
+    <t>Lhub_SRS_2.4.2.8</t>
+  </si>
+  <si>
+    <t>Lhub_SRS_2.4.2.9</t>
+  </si>
+  <si>
+    <t>Lhub_SRS_2.4.2.10</t>
+  </si>
+  <si>
+    <t>Lhub_SRS_2.4.2.11</t>
+  </si>
+  <si>
+    <t>Lhub_SRS_2.4.2.12</t>
+  </si>
+  <si>
+    <t>Lhub_SRS_2.4.2.13</t>
+  </si>
+  <si>
+    <t>Lhub_SRS_2.4.3.7</t>
+  </si>
+  <si>
+    <t>Lhub_SRS_2.4.3.8</t>
+  </si>
+  <si>
+    <t>Lhub_SRS_2.4.3.9</t>
+  </si>
+  <si>
+    <t>Lhub_SRS_2.4.5.2</t>
+  </si>
+  <si>
+    <t>Lhub_SRS_2.4.5.3</t>
+  </si>
+  <si>
+    <t>Lhub_SRS_2.4.5.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Changes in SRS IDs </t>
+  </si>
+  <si>
+    <t>Aya</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="16">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -255,6 +348,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="16"/>
@@ -309,11 +403,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Century Gothic"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <name val="Montserrat"/>
     </font>
     <font>
@@ -343,8 +432,37 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="16"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -381,8 +499,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -405,170 +529,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -589,170 +556,112 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="15" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -1078,91 +987,98 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z34"/>
+  <dimension ref="A1:Z65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.33203125" style="16" customWidth="1"/>
-    <col min="2" max="2" width="30.44140625" style="16" customWidth="1"/>
-    <col min="3" max="3" width="48.109375" style="16" customWidth="1"/>
-    <col min="4" max="4" width="23.33203125" style="16" customWidth="1"/>
-    <col min="5" max="5" width="35.88671875" style="16" customWidth="1"/>
-    <col min="6" max="6" width="38" style="16" customWidth="1"/>
-    <col min="7" max="7" width="37.5546875" style="16" customWidth="1"/>
-    <col min="8" max="8" width="44.5546875" style="16" customWidth="1"/>
-    <col min="9" max="16384" width="9.109375" style="16"/>
+    <col min="1" max="1" width="23.28515625" style="12" customWidth="1"/>
+    <col min="2" max="2" width="30.42578125" style="12" customWidth="1"/>
+    <col min="3" max="3" width="48.140625" style="12" customWidth="1"/>
+    <col min="4" max="4" width="23.28515625" style="12" customWidth="1"/>
+    <col min="5" max="5" width="35.85546875" style="12" customWidth="1"/>
+    <col min="6" max="6" width="38" style="22" customWidth="1"/>
+    <col min="7" max="7" width="37.5703125" style="12" customWidth="1"/>
+    <col min="8" max="8" width="44.5703125" style="12" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1">
+    <row r="1" spans="1:26" s="4" customFormat="1" ht="30" customHeight="1">
+      <c r="F1" s="20"/>
       <c r="H1" s="4" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:26" s="5" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="30" t="s">
+      <c r="C2" s="25"/>
+      <c r="D2" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="E2" s="31" t="s">
+      <c r="E2" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="F2" s="31" t="s">
+      <c r="F2" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="G2" s="31" t="s">
+      <c r="G2" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="H2" s="32" t="s">
+      <c r="H2" s="28" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:26" s="5" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="46"/>
-      <c r="D3" s="33" t="s">
+      <c r="C3" s="25"/>
+      <c r="D3" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="E3" s="29">
+      <c r="E3" s="14">
         <v>43588</v>
       </c>
-      <c r="F3" s="29">
+      <c r="F3" s="14">
         <v>43529</v>
       </c>
-      <c r="G3" s="34" t="s">
+      <c r="G3" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="H3" s="35" t="s">
+      <c r="H3" s="15" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:26" s="5" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
-      <c r="A4" s="39" t="s">
+    <row r="4" spans="1:26" s="5" customFormat="1" ht="23.25" customHeight="1">
+      <c r="A4" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="47">
+      <c r="B4" s="26">
         <v>43470</v>
       </c>
-      <c r="C4" s="47"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="38"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="14">
+        <v>43592</v>
+      </c>
+      <c r="F4" s="31"/>
+      <c r="G4" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="5" spans="1:26" s="7" customFormat="1" ht="33.75" customHeight="1">
       <c r="A5" s="1" t="s">
@@ -1209,22 +1125,22 @@
       <c r="Z5" s="6"/>
     </row>
     <row r="6" spans="1:26" s="9" customFormat="1" ht="24.75" customHeight="1">
-      <c r="A6" s="40">
+      <c r="A6" s="23">
         <v>1</v>
       </c>
-      <c r="B6" s="48" t="s">
+      <c r="B6" s="27" t="s">
         <v>32</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="41"/>
-      <c r="E6" s="17" t="s">
+      <c r="D6" s="24"/>
+      <c r="E6" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42"/>
-      <c r="H6" s="42"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
       <c r="K6" s="8"/>
@@ -1245,18 +1161,18 @@
       <c r="Z6" s="8"/>
     </row>
     <row r="7" spans="1:26" s="9" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A7" s="40"/>
-      <c r="B7" s="48"/>
+      <c r="A7" s="23"/>
+      <c r="B7" s="27"/>
       <c r="C7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="41"/>
-      <c r="E7" s="13" t="s">
+      <c r="D7" s="24"/>
+      <c r="E7" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="43"/>
-      <c r="G7" s="43"/>
-      <c r="H7" s="43"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32"/>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
       <c r="K7" s="8"/>
@@ -1276,55 +1192,53 @@
       <c r="Y7" s="8"/>
       <c r="Z7" s="8"/>
     </row>
-    <row r="8" spans="1:26" s="9" customFormat="1" ht="18" customHeight="1">
-      <c r="A8" s="44">
+    <row r="8" spans="1:26" s="43" customFormat="1" ht="3.75" customHeight="1">
+      <c r="A8" s="37"/>
+      <c r="B8" s="38"/>
+      <c r="C8" s="39"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="42"/>
+      <c r="J8" s="42"/>
+      <c r="K8" s="42"/>
+      <c r="L8" s="42"/>
+      <c r="M8" s="42"/>
+      <c r="N8" s="42"/>
+      <c r="O8" s="42"/>
+      <c r="P8" s="42"/>
+      <c r="Q8" s="42"/>
+      <c r="R8" s="42"/>
+      <c r="S8" s="42"/>
+      <c r="T8" s="42"/>
+      <c r="U8" s="42"/>
+      <c r="V8" s="42"/>
+      <c r="W8" s="42"/>
+      <c r="X8" s="42"/>
+      <c r="Y8" s="42"/>
+      <c r="Z8" s="42"/>
+    </row>
+    <row r="9" spans="1:26" s="9" customFormat="1" ht="18" customHeight="1">
+      <c r="A9" s="23">
         <v>2</v>
       </c>
-      <c r="B8" s="49" t="s">
+      <c r="B9" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="53"/>
-      <c r="E8" s="13" t="s">
+      <c r="D9" s="24"/>
+      <c r="E9" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="F8" s="56"/>
-      <c r="G8" s="44"/>
-      <c r="H8" s="44"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
-      <c r="P8" s="8"/>
-      <c r="Q8" s="8"/>
-      <c r="R8" s="8"/>
-      <c r="S8" s="8"/>
-      <c r="T8" s="8"/>
-      <c r="U8" s="8"/>
-      <c r="V8" s="8"/>
-      <c r="W8" s="8"/>
-      <c r="X8" s="8"/>
-      <c r="Y8" s="8"/>
-      <c r="Z8" s="8"/>
-    </row>
-    <row r="9" spans="1:26" s="9" customFormat="1" ht="21" customHeight="1">
-      <c r="A9" s="52"/>
-      <c r="B9" s="50"/>
-      <c r="C9" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="54"/>
-      <c r="E9" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F9" s="57"/>
-      <c r="G9" s="45"/>
-      <c r="H9" s="45"/>
+      <c r="F9" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
@@ -1344,19 +1258,19 @@
       <c r="Y9" s="8"/>
       <c r="Z9" s="8"/>
     </row>
-    <row r="10" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A10" s="52"/>
-      <c r="B10" s="50"/>
-      <c r="C10" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="54"/>
-      <c r="E10" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="F10" s="57"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="15"/>
+    <row r="10" spans="1:26" s="9" customFormat="1" ht="21" customHeight="1">
+      <c r="A10" s="23"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="24"/>
+      <c r="E10" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="33"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="23"/>
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
       <c r="K10" s="8"/>
@@ -1377,18 +1291,18 @@
       <c r="Z10" s="8"/>
     </row>
     <row r="11" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A11" s="52"/>
-      <c r="B11" s="50"/>
-      <c r="C11" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="D11" s="54"/>
-      <c r="E11" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="F11" s="57"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="15"/>
+      <c r="A11" s="23"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="24"/>
+      <c r="E11" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" s="33"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="11"/>
       <c r="I11" s="8"/>
       <c r="J11" s="8"/>
       <c r="K11" s="8"/>
@@ -1409,16 +1323,18 @@
       <c r="Z11" s="8"/>
     </row>
     <row r="12" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A12" s="52"/>
-      <c r="B12" s="50"/>
-      <c r="C12" s="59"/>
-      <c r="D12" s="54"/>
-      <c r="E12" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="F12" s="57"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="15"/>
+      <c r="A12" s="23"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" s="24"/>
+      <c r="E12" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" s="33"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="11"/>
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>
@@ -1439,16 +1355,16 @@
       <c r="Z12" s="8"/>
     </row>
     <row r="13" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A13" s="52"/>
-      <c r="B13" s="50"/>
-      <c r="C13" s="59"/>
-      <c r="D13" s="54"/>
-      <c r="E13" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="F13" s="57"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="15"/>
+      <c r="A13" s="23"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F13" s="33"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="11"/>
       <c r="I13" s="8"/>
       <c r="J13" s="8"/>
       <c r="K13" s="8"/>
@@ -1469,16 +1385,16 @@
       <c r="Z13" s="8"/>
     </row>
     <row r="14" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A14" s="52"/>
-      <c r="B14" s="50"/>
-      <c r="C14" s="59"/>
-      <c r="D14" s="54"/>
-      <c r="E14" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="F14" s="57"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="15"/>
+      <c r="A14" s="23"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="34"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="F14" s="33"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="11"/>
       <c r="I14" s="8"/>
       <c r="J14" s="8"/>
       <c r="K14" s="8"/>
@@ -1499,16 +1415,16 @@
       <c r="Z14" s="8"/>
     </row>
     <row r="15" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A15" s="45"/>
-      <c r="B15" s="51"/>
-      <c r="C15" s="60"/>
-      <c r="D15" s="55"/>
-      <c r="E15" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="F15" s="58"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="15"/>
+      <c r="A15" s="23"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="F15" s="33"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="11"/>
       <c r="I15" s="8"/>
       <c r="J15" s="8"/>
       <c r="K15" s="8"/>
@@ -1528,22 +1444,17 @@
       <c r="Y15" s="8"/>
       <c r="Z15" s="8"/>
     </row>
-    <row r="16" spans="1:26" s="9" customFormat="1" ht="27" customHeight="1">
-      <c r="A16" s="44">
-        <v>3</v>
-      </c>
-      <c r="B16" s="49" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E16" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="F16" s="14"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="15"/>
+    <row r="16" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A16" s="23"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="F16" s="33"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="11"/>
       <c r="I16" s="8"/>
       <c r="J16" s="8"/>
       <c r="K16" s="8"/>
@@ -1563,16 +1474,17 @@
       <c r="Y16" s="8"/>
       <c r="Z16" s="8"/>
     </row>
-    <row r="17" spans="1:26" s="9" customFormat="1" ht="27" customHeight="1">
-      <c r="A17" s="52"/>
-      <c r="B17" s="50"/>
-      <c r="C17" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E17" s="27"/>
-      <c r="F17" s="61"/>
-      <c r="G17" s="28"/>
-      <c r="H17" s="15"/>
+    <row r="17" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A17" s="23"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="F17" s="33"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="11"/>
       <c r="I17" s="8"/>
       <c r="J17" s="8"/>
       <c r="K17" s="8"/>
@@ -1592,16 +1504,17 @@
       <c r="Y17" s="8"/>
       <c r="Z17" s="8"/>
     </row>
-    <row r="18" spans="1:26" s="9" customFormat="1" ht="27" customHeight="1">
-      <c r="A18" s="52"/>
-      <c r="B18" s="50"/>
-      <c r="C18" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E18" s="27"/>
-      <c r="F18" s="61"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="15"/>
+    <row r="18" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A18" s="23"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="F18" s="33"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="11"/>
       <c r="I18" s="8"/>
       <c r="J18" s="8"/>
       <c r="K18" s="8"/>
@@ -1621,17 +1534,17 @@
       <c r="Y18" s="8"/>
       <c r="Z18" s="8"/>
     </row>
-    <row r="19" spans="1:26" s="9" customFormat="1" ht="27" customHeight="1">
-      <c r="A19" s="52"/>
-      <c r="B19" s="50"/>
-      <c r="C19" s="3" t="s">
-        <v>22</v>
-      </c>
+    <row r="19" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A19" s="23"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="34"/>
       <c r="D19" s="24"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="61"/>
-      <c r="G19" s="28"/>
-      <c r="H19" s="15"/>
+      <c r="E19" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="F19" s="33"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="11"/>
       <c r="I19" s="8"/>
       <c r="J19" s="8"/>
       <c r="K19" s="8"/>
@@ -1651,17 +1564,17 @@
       <c r="Y19" s="8"/>
       <c r="Z19" s="8"/>
     </row>
-    <row r="20" spans="1:26" s="9" customFormat="1" ht="27" customHeight="1">
-      <c r="A20" s="45"/>
-      <c r="B20" s="51"/>
-      <c r="C20" s="3" t="s">
-        <v>23</v>
-      </c>
+    <row r="20" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A20" s="23"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="34"/>
       <c r="D20" s="24"/>
-      <c r="E20" s="27"/>
-      <c r="F20" s="61"/>
-      <c r="G20" s="28"/>
-      <c r="H20" s="15"/>
+      <c r="E20" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="F20" s="33"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="11"/>
       <c r="I20" s="8"/>
       <c r="J20" s="8"/>
       <c r="K20" s="8"/>
@@ -1681,23 +1594,17 @@
       <c r="Y20" s="8"/>
       <c r="Z20" s="8"/>
     </row>
-    <row r="21" spans="1:26" s="9" customFormat="1" ht="21.75" customHeight="1">
-      <c r="A21" s="44">
-        <v>4</v>
-      </c>
-      <c r="B21" s="49" t="s">
-        <v>35</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D21" s="53"/>
-      <c r="E21" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="F21" s="18"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="15"/>
+    <row r="21" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A21" s="23"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="F21" s="33"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="11"/>
       <c r="I21" s="8"/>
       <c r="J21" s="8"/>
       <c r="K21" s="8"/>
@@ -1717,19 +1624,17 @@
       <c r="Y21" s="8"/>
       <c r="Z21" s="8"/>
     </row>
-    <row r="22" spans="1:26" s="9" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A22" s="52"/>
-      <c r="B22" s="50"/>
-      <c r="C22" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D22" s="54"/>
-      <c r="E22" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="F22" s="19"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="15"/>
+    <row r="22" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A22" s="23"/>
+      <c r="B22" s="27"/>
+      <c r="C22" s="34"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="F22" s="33"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="11"/>
       <c r="I22" s="8"/>
       <c r="J22" s="8"/>
       <c r="K22" s="8"/>
@@ -1750,16 +1655,16 @@
       <c r="Z22" s="8"/>
     </row>
     <row r="23" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A23" s="52"/>
-      <c r="B23" s="50"/>
-      <c r="C23" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D23" s="54"/>
-      <c r="E23" s="63"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="22"/>
-      <c r="H23" s="15"/>
+      <c r="A23" s="23"/>
+      <c r="B23" s="27"/>
+      <c r="C23" s="34"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F23" s="33"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="11"/>
       <c r="I23" s="8"/>
       <c r="J23" s="8"/>
       <c r="K23" s="8"/>
@@ -1780,14 +1685,16 @@
       <c r="Z23" s="8"/>
     </row>
     <row r="24" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A24" s="52"/>
-      <c r="B24" s="50"/>
-      <c r="C24" s="62"/>
-      <c r="D24" s="54"/>
-      <c r="E24" s="64"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="22"/>
-      <c r="H24" s="15"/>
+      <c r="A24" s="23"/>
+      <c r="B24" s="27"/>
+      <c r="C24" s="34"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F24" s="33"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="11"/>
       <c r="I24" s="8"/>
       <c r="J24" s="8"/>
       <c r="K24" s="8"/>
@@ -1807,15 +1714,17 @@
       <c r="Y24" s="8"/>
       <c r="Z24" s="8"/>
     </row>
-    <row r="25" spans="1:26" s="9" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A25" s="45"/>
-      <c r="B25" s="51"/>
-      <c r="C25" s="60"/>
-      <c r="D25" s="55"/>
-      <c r="E25" s="65"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="23"/>
-      <c r="H25" s="15"/>
+    <row r="25" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A25" s="23"/>
+      <c r="B25" s="27"/>
+      <c r="C25" s="34"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F25" s="33"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="11"/>
       <c r="I25" s="8"/>
       <c r="J25" s="8"/>
       <c r="K25" s="8"/>
@@ -1835,22 +1744,17 @@
       <c r="Y25" s="8"/>
       <c r="Z25" s="8"/>
     </row>
-    <row r="26" spans="1:26" s="9" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A26" s="44">
-        <v>5</v>
-      </c>
-      <c r="B26" s="49" t="s">
-        <v>36</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E26" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="F26" s="14"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="15"/>
+    <row r="26" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A26" s="23"/>
+      <c r="B26" s="27"/>
+      <c r="C26" s="34"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="F26" s="33"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="11"/>
       <c r="I26" s="8"/>
       <c r="J26" s="8"/>
       <c r="K26" s="8"/>
@@ -1870,16 +1774,17 @@
       <c r="Y26" s="8"/>
       <c r="Z26" s="8"/>
     </row>
-    <row r="27" spans="1:26" s="9" customFormat="1" ht="21" customHeight="1">
-      <c r="A27" s="52"/>
-      <c r="B27" s="50"/>
-      <c r="C27" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E27" s="13"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="15"/>
+    <row r="27" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A27" s="23"/>
+      <c r="B27" s="27"/>
+      <c r="C27" s="34"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="F27" s="33"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="11"/>
       <c r="I27" s="8"/>
       <c r="J27" s="8"/>
       <c r="K27" s="8"/>
@@ -1899,16 +1804,17 @@
       <c r="Y27" s="8"/>
       <c r="Z27" s="8"/>
     </row>
-    <row r="28" spans="1:26" s="9" customFormat="1" ht="21" customHeight="1">
-      <c r="A28" s="45"/>
-      <c r="B28" s="51"/>
-      <c r="C28" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E28" s="13"/>
-      <c r="F28" s="14"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="15"/>
+    <row r="28" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A28" s="18"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="F28" s="21"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="11"/>
       <c r="I28" s="8"/>
       <c r="J28" s="8"/>
       <c r="K28" s="8"/>
@@ -1928,23 +1834,17 @@
       <c r="Y28" s="8"/>
       <c r="Z28" s="8"/>
     </row>
-    <row r="29" spans="1:26" s="9" customFormat="1" ht="21" customHeight="1">
-      <c r="A29" s="44">
-        <v>6</v>
-      </c>
-      <c r="B29" s="49" t="s">
-        <v>37</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D29" s="53"/>
-      <c r="E29" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="F29" s="14"/>
-      <c r="G29" s="10"/>
-      <c r="H29" s="15"/>
+    <row r="29" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A29" s="18"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="F29" s="21"/>
+      <c r="G29" s="18"/>
+      <c r="H29" s="11"/>
       <c r="I29" s="8"/>
       <c r="J29" s="8"/>
       <c r="K29" s="8"/>
@@ -1964,17 +1864,17 @@
       <c r="Y29" s="8"/>
       <c r="Z29" s="8"/>
     </row>
-    <row r="30" spans="1:26" s="9" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A30" s="52"/>
-      <c r="B30" s="50"/>
-      <c r="C30" s="62"/>
-      <c r="D30" s="54"/>
-      <c r="E30" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="F30" s="14"/>
-      <c r="G30" s="10"/>
-      <c r="H30" s="15"/>
+    <row r="30" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A30" s="18"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="F30" s="21"/>
+      <c r="G30" s="18"/>
+      <c r="H30" s="11"/>
       <c r="I30" s="8"/>
       <c r="J30" s="8"/>
       <c r="K30" s="8"/>
@@ -1994,17 +1894,17 @@
       <c r="Y30" s="8"/>
       <c r="Z30" s="8"/>
     </row>
-    <row r="31" spans="1:26" s="9" customFormat="1" ht="21" customHeight="1">
-      <c r="A31" s="52"/>
-      <c r="B31" s="50"/>
-      <c r="C31" s="59"/>
-      <c r="D31" s="54"/>
-      <c r="E31" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="F31" s="14"/>
-      <c r="G31" s="10"/>
-      <c r="H31" s="15"/>
+    <row r="31" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A31" s="18"/>
+      <c r="B31" s="17"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="F31" s="21"/>
+      <c r="G31" s="18"/>
+      <c r="H31" s="11"/>
       <c r="I31" s="8"/>
       <c r="J31" s="8"/>
       <c r="K31" s="8"/>
@@ -2024,21 +1924,17 @@
       <c r="Y31" s="8"/>
       <c r="Z31" s="8"/>
     </row>
-    <row r="32" spans="1:26" s="9" customFormat="1" ht="33" customHeight="1">
-      <c r="A32" s="10">
-        <v>7</v>
-      </c>
-      <c r="B32" s="11" t="s">
-        <v>38</v>
-      </c>
+    <row r="32" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A32" s="18"/>
+      <c r="B32" s="17"/>
       <c r="C32" s="3"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="F32" s="14"/>
-      <c r="G32" s="10"/>
-      <c r="H32" s="15"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="F32" s="21"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="11"/>
       <c r="I32" s="8"/>
       <c r="J32" s="8"/>
       <c r="K32" s="8"/>
@@ -2058,23 +1954,17 @@
       <c r="Y32" s="8"/>
       <c r="Z32" s="8"/>
     </row>
-    <row r="33" spans="1:26" s="9" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A33" s="10">
-        <v>8</v>
-      </c>
-      <c r="B33" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D33" s="12"/>
-      <c r="E33" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="F33" s="14"/>
-      <c r="G33" s="10"/>
-      <c r="H33" s="15"/>
+    <row r="33" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A33" s="18"/>
+      <c r="B33" s="17"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="F33" s="21"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="11"/>
       <c r="I33" s="8"/>
       <c r="J33" s="8"/>
       <c r="K33" s="8"/>
@@ -2094,21 +1984,17 @@
       <c r="Y33" s="8"/>
       <c r="Z33" s="8"/>
     </row>
-    <row r="34" spans="1:26" s="9" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A34" s="10">
-        <v>9</v>
-      </c>
-      <c r="B34" s="25" t="s">
-        <v>57</v>
-      </c>
+    <row r="34" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A34" s="18"/>
+      <c r="B34" s="17"/>
       <c r="C34" s="3"/>
-      <c r="D34" s="12"/>
-      <c r="E34" s="27" t="s">
-        <v>58</v>
-      </c>
-      <c r="F34" s="14"/>
-      <c r="G34" s="10"/>
-      <c r="H34" s="15"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="F34" s="21"/>
+      <c r="G34" s="18"/>
+      <c r="H34" s="11"/>
       <c r="I34" s="8"/>
       <c r="J34" s="8"/>
       <c r="K34" s="8"/>
@@ -2128,32 +2014,996 @@
       <c r="Y34" s="8"/>
       <c r="Z34" s="8"/>
     </row>
+    <row r="35" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A35" s="18"/>
+      <c r="B35" s="17"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="19"/>
+      <c r="E35" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="F35" s="21"/>
+      <c r="G35" s="18"/>
+      <c r="H35" s="11"/>
+      <c r="I35" s="8"/>
+      <c r="J35" s="8"/>
+      <c r="K35" s="8"/>
+      <c r="L35" s="8"/>
+      <c r="M35" s="8"/>
+      <c r="N35" s="8"/>
+      <c r="O35" s="8"/>
+      <c r="P35" s="8"/>
+      <c r="Q35" s="8"/>
+      <c r="R35" s="8"/>
+      <c r="S35" s="8"/>
+      <c r="T35" s="8"/>
+      <c r="U35" s="8"/>
+      <c r="V35" s="8"/>
+      <c r="W35" s="8"/>
+      <c r="X35" s="8"/>
+      <c r="Y35" s="8"/>
+      <c r="Z35" s="8"/>
+    </row>
+    <row r="36" spans="1:26" s="43" customFormat="1" ht="3.75" customHeight="1">
+      <c r="A36" s="37"/>
+      <c r="B36" s="38"/>
+      <c r="C36" s="39"/>
+      <c r="D36" s="40"/>
+      <c r="E36" s="41"/>
+      <c r="F36" s="44"/>
+      <c r="G36" s="37"/>
+      <c r="H36" s="45"/>
+      <c r="I36" s="42"/>
+      <c r="J36" s="42"/>
+      <c r="K36" s="42"/>
+      <c r="L36" s="42"/>
+      <c r="M36" s="42"/>
+      <c r="N36" s="42"/>
+      <c r="O36" s="42"/>
+      <c r="P36" s="42"/>
+      <c r="Q36" s="42"/>
+      <c r="R36" s="42"/>
+      <c r="S36" s="42"/>
+      <c r="T36" s="42"/>
+      <c r="U36" s="42"/>
+      <c r="V36" s="42"/>
+      <c r="W36" s="42"/>
+      <c r="X36" s="42"/>
+      <c r="Y36" s="42"/>
+      <c r="Z36" s="42"/>
+    </row>
+    <row r="37" spans="1:26" s="9" customFormat="1" ht="27" customHeight="1">
+      <c r="A37" s="23">
+        <v>3</v>
+      </c>
+      <c r="B37" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E37" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="F37" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="G37" s="18"/>
+      <c r="H37" s="11"/>
+      <c r="I37" s="8"/>
+      <c r="J37" s="8"/>
+      <c r="K37" s="8"/>
+      <c r="L37" s="8"/>
+      <c r="M37" s="8"/>
+      <c r="N37" s="8"/>
+      <c r="O37" s="8"/>
+      <c r="P37" s="8"/>
+      <c r="Q37" s="8"/>
+      <c r="R37" s="8"/>
+      <c r="S37" s="8"/>
+      <c r="T37" s="8"/>
+      <c r="U37" s="8"/>
+      <c r="V37" s="8"/>
+      <c r="W37" s="8"/>
+      <c r="X37" s="8"/>
+      <c r="Y37" s="8"/>
+      <c r="Z37" s="8"/>
+    </row>
+    <row r="38" spans="1:26" s="9" customFormat="1" ht="27" customHeight="1">
+      <c r="A38" s="23"/>
+      <c r="B38" s="27"/>
+      <c r="C38" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E38" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="F38" s="21"/>
+      <c r="G38" s="18"/>
+      <c r="H38" s="11"/>
+      <c r="I38" s="8"/>
+      <c r="J38" s="8"/>
+      <c r="K38" s="8"/>
+      <c r="L38" s="8"/>
+      <c r="M38" s="8"/>
+      <c r="N38" s="8"/>
+      <c r="O38" s="8"/>
+      <c r="P38" s="8"/>
+      <c r="Q38" s="8"/>
+      <c r="R38" s="8"/>
+      <c r="S38" s="8"/>
+      <c r="T38" s="8"/>
+      <c r="U38" s="8"/>
+      <c r="V38" s="8"/>
+      <c r="W38" s="8"/>
+      <c r="X38" s="8"/>
+      <c r="Y38" s="8"/>
+      <c r="Z38" s="8"/>
+    </row>
+    <row r="39" spans="1:26" s="9" customFormat="1" ht="27" customHeight="1">
+      <c r="A39" s="23"/>
+      <c r="B39" s="27"/>
+      <c r="C39" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E39" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="F39" s="21"/>
+      <c r="G39" s="18"/>
+      <c r="H39" s="11"/>
+      <c r="I39" s="8"/>
+      <c r="J39" s="8"/>
+      <c r="K39" s="8"/>
+      <c r="L39" s="8"/>
+      <c r="M39" s="8"/>
+      <c r="N39" s="8"/>
+      <c r="O39" s="8"/>
+      <c r="P39" s="8"/>
+      <c r="Q39" s="8"/>
+      <c r="R39" s="8"/>
+      <c r="S39" s="8"/>
+      <c r="T39" s="8"/>
+      <c r="U39" s="8"/>
+      <c r="V39" s="8"/>
+      <c r="W39" s="8"/>
+      <c r="X39" s="8"/>
+      <c r="Y39" s="8"/>
+      <c r="Z39" s="8"/>
+    </row>
+    <row r="40" spans="1:26" s="9" customFormat="1" ht="27" customHeight="1">
+      <c r="A40" s="23"/>
+      <c r="B40" s="27"/>
+      <c r="C40" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D40" s="3"/>
+      <c r="E40" s="35" t="s">
+        <v>51</v>
+      </c>
+      <c r="F40" s="21"/>
+      <c r="G40" s="18"/>
+      <c r="H40" s="11"/>
+      <c r="I40" s="8"/>
+      <c r="J40" s="8"/>
+      <c r="K40" s="8"/>
+      <c r="L40" s="8"/>
+      <c r="M40" s="8"/>
+      <c r="N40" s="8"/>
+      <c r="O40" s="8"/>
+      <c r="P40" s="8"/>
+      <c r="Q40" s="8"/>
+      <c r="R40" s="8"/>
+      <c r="S40" s="8"/>
+      <c r="T40" s="8"/>
+      <c r="U40" s="8"/>
+      <c r="V40" s="8"/>
+      <c r="W40" s="8"/>
+      <c r="X40" s="8"/>
+      <c r="Y40" s="8"/>
+      <c r="Z40" s="8"/>
+    </row>
+    <row r="41" spans="1:26" s="9" customFormat="1" ht="27" customHeight="1">
+      <c r="A41" s="23"/>
+      <c r="B41" s="27"/>
+      <c r="C41" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D41" s="3"/>
+      <c r="E41" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="F41" s="21"/>
+      <c r="G41" s="18"/>
+      <c r="H41" s="11"/>
+      <c r="I41" s="8"/>
+      <c r="J41" s="8"/>
+      <c r="K41" s="8"/>
+      <c r="L41" s="8"/>
+      <c r="M41" s="8"/>
+      <c r="N41" s="8"/>
+      <c r="O41" s="8"/>
+      <c r="P41" s="8"/>
+      <c r="Q41" s="8"/>
+      <c r="R41" s="8"/>
+      <c r="S41" s="8"/>
+      <c r="T41" s="8"/>
+      <c r="U41" s="8"/>
+      <c r="V41" s="8"/>
+      <c r="W41" s="8"/>
+      <c r="X41" s="8"/>
+      <c r="Y41" s="8"/>
+      <c r="Z41" s="8"/>
+    </row>
+    <row r="42" spans="1:26" s="9" customFormat="1" ht="27" customHeight="1">
+      <c r="A42" s="18"/>
+      <c r="B42" s="17"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="F42" s="21"/>
+      <c r="G42" s="18"/>
+      <c r="H42" s="11"/>
+      <c r="I42" s="8"/>
+      <c r="J42" s="8"/>
+      <c r="K42" s="8"/>
+      <c r="L42" s="8"/>
+      <c r="M42" s="8"/>
+      <c r="N42" s="8"/>
+      <c r="O42" s="8"/>
+      <c r="P42" s="8"/>
+      <c r="Q42" s="8"/>
+      <c r="R42" s="8"/>
+      <c r="S42" s="8"/>
+      <c r="T42" s="8"/>
+      <c r="U42" s="8"/>
+      <c r="V42" s="8"/>
+      <c r="W42" s="8"/>
+      <c r="X42" s="8"/>
+      <c r="Y42" s="8"/>
+      <c r="Z42" s="8"/>
+    </row>
+    <row r="43" spans="1:26" s="43" customFormat="1" ht="3.75" customHeight="1">
+      <c r="A43" s="37"/>
+      <c r="B43" s="38"/>
+      <c r="C43" s="39"/>
+      <c r="D43" s="40"/>
+      <c r="E43" s="41"/>
+      <c r="F43" s="44"/>
+      <c r="G43" s="37"/>
+      <c r="H43" s="45"/>
+      <c r="I43" s="42"/>
+      <c r="J43" s="42"/>
+      <c r="K43" s="42"/>
+      <c r="L43" s="42"/>
+      <c r="M43" s="42"/>
+      <c r="N43" s="42"/>
+      <c r="O43" s="42"/>
+      <c r="P43" s="42"/>
+      <c r="Q43" s="42"/>
+      <c r="R43" s="42"/>
+      <c r="S43" s="42"/>
+      <c r="T43" s="42"/>
+      <c r="U43" s="42"/>
+      <c r="V43" s="42"/>
+      <c r="W43" s="42"/>
+      <c r="X43" s="42"/>
+      <c r="Y43" s="42"/>
+      <c r="Z43" s="42"/>
+    </row>
+    <row r="44" spans="1:26" s="9" customFormat="1" ht="21.75" customHeight="1">
+      <c r="A44" s="23">
+        <v>4</v>
+      </c>
+      <c r="B44" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D44" s="24"/>
+      <c r="E44" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="F44" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="G44" s="11"/>
+      <c r="H44" s="11"/>
+      <c r="I44" s="8"/>
+      <c r="J44" s="8"/>
+      <c r="K44" s="8"/>
+      <c r="L44" s="8"/>
+      <c r="M44" s="8"/>
+      <c r="N44" s="8"/>
+      <c r="O44" s="8"/>
+      <c r="P44" s="8"/>
+      <c r="Q44" s="8"/>
+      <c r="R44" s="8"/>
+      <c r="S44" s="8"/>
+      <c r="T44" s="8"/>
+      <c r="U44" s="8"/>
+      <c r="V44" s="8"/>
+      <c r="W44" s="8"/>
+      <c r="X44" s="8"/>
+      <c r="Y44" s="8"/>
+      <c r="Z44" s="8"/>
+    </row>
+    <row r="45" spans="1:26" s="9" customFormat="1" ht="23.25" customHeight="1">
+      <c r="A45" s="23"/>
+      <c r="B45" s="27"/>
+      <c r="C45" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D45" s="24"/>
+      <c r="E45" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="F45" s="21"/>
+      <c r="G45" s="11"/>
+      <c r="H45" s="11"/>
+      <c r="I45" s="8"/>
+      <c r="J45" s="8"/>
+      <c r="K45" s="8"/>
+      <c r="L45" s="8"/>
+      <c r="M45" s="8"/>
+      <c r="N45" s="8"/>
+      <c r="O45" s="8"/>
+      <c r="P45" s="8"/>
+      <c r="Q45" s="8"/>
+      <c r="R45" s="8"/>
+      <c r="S45" s="8"/>
+      <c r="T45" s="8"/>
+      <c r="U45" s="8"/>
+      <c r="V45" s="8"/>
+      <c r="W45" s="8"/>
+      <c r="X45" s="8"/>
+      <c r="Y45" s="8"/>
+      <c r="Z45" s="8"/>
+    </row>
+    <row r="46" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A46" s="23"/>
+      <c r="B46" s="27"/>
+      <c r="C46" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D46" s="24"/>
+      <c r="E46" s="36"/>
+      <c r="F46" s="21"/>
+      <c r="G46" s="11"/>
+      <c r="H46" s="11"/>
+      <c r="I46" s="8"/>
+      <c r="J46" s="8"/>
+      <c r="K46" s="8"/>
+      <c r="L46" s="8"/>
+      <c r="M46" s="8"/>
+      <c r="N46" s="8"/>
+      <c r="O46" s="8"/>
+      <c r="P46" s="8"/>
+      <c r="Q46" s="8"/>
+      <c r="R46" s="8"/>
+      <c r="S46" s="8"/>
+      <c r="T46" s="8"/>
+      <c r="U46" s="8"/>
+      <c r="V46" s="8"/>
+      <c r="W46" s="8"/>
+      <c r="X46" s="8"/>
+      <c r="Y46" s="8"/>
+      <c r="Z46" s="8"/>
+    </row>
+    <row r="47" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A47" s="23"/>
+      <c r="B47" s="27"/>
+      <c r="C47" s="34"/>
+      <c r="D47" s="24"/>
+      <c r="E47" s="36"/>
+      <c r="F47" s="21"/>
+      <c r="G47" s="11"/>
+      <c r="H47" s="11"/>
+      <c r="I47" s="8"/>
+      <c r="J47" s="8"/>
+      <c r="K47" s="8"/>
+      <c r="L47" s="8"/>
+      <c r="M47" s="8"/>
+      <c r="N47" s="8"/>
+      <c r="O47" s="8"/>
+      <c r="P47" s="8"/>
+      <c r="Q47" s="8"/>
+      <c r="R47" s="8"/>
+      <c r="S47" s="8"/>
+      <c r="T47" s="8"/>
+      <c r="U47" s="8"/>
+      <c r="V47" s="8"/>
+      <c r="W47" s="8"/>
+      <c r="X47" s="8"/>
+      <c r="Y47" s="8"/>
+      <c r="Z47" s="8"/>
+    </row>
+    <row r="48" spans="1:26" s="9" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A48" s="23"/>
+      <c r="B48" s="27"/>
+      <c r="C48" s="34"/>
+      <c r="D48" s="24"/>
+      <c r="E48" s="36"/>
+      <c r="F48" s="21"/>
+      <c r="G48" s="11"/>
+      <c r="H48" s="11"/>
+      <c r="I48" s="8"/>
+      <c r="J48" s="8"/>
+      <c r="K48" s="8"/>
+      <c r="L48" s="8"/>
+      <c r="M48" s="8"/>
+      <c r="N48" s="8"/>
+      <c r="O48" s="8"/>
+      <c r="P48" s="8"/>
+      <c r="Q48" s="8"/>
+      <c r="R48" s="8"/>
+      <c r="S48" s="8"/>
+      <c r="T48" s="8"/>
+      <c r="U48" s="8"/>
+      <c r="V48" s="8"/>
+      <c r="W48" s="8"/>
+      <c r="X48" s="8"/>
+      <c r="Y48" s="8"/>
+      <c r="Z48" s="8"/>
+    </row>
+    <row r="49" spans="1:26" s="43" customFormat="1" ht="3.75" customHeight="1">
+      <c r="A49" s="37"/>
+      <c r="B49" s="38"/>
+      <c r="C49" s="39"/>
+      <c r="D49" s="40"/>
+      <c r="E49" s="41"/>
+      <c r="F49" s="44"/>
+      <c r="G49" s="37"/>
+      <c r="H49" s="45"/>
+      <c r="I49" s="42"/>
+      <c r="J49" s="42"/>
+      <c r="K49" s="42"/>
+      <c r="L49" s="42"/>
+      <c r="M49" s="42"/>
+      <c r="N49" s="42"/>
+      <c r="O49" s="42"/>
+      <c r="P49" s="42"/>
+      <c r="Q49" s="42"/>
+      <c r="R49" s="42"/>
+      <c r="S49" s="42"/>
+      <c r="T49" s="42"/>
+      <c r="U49" s="42"/>
+      <c r="V49" s="42"/>
+      <c r="W49" s="42"/>
+      <c r="X49" s="42"/>
+      <c r="Y49" s="42"/>
+      <c r="Z49" s="42"/>
+    </row>
+    <row r="50" spans="1:26" s="9" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A50" s="23">
+        <v>5</v>
+      </c>
+      <c r="B50" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E50" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="F50" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="G50" s="18"/>
+      <c r="H50" s="11"/>
+      <c r="I50" s="8"/>
+      <c r="J50" s="8"/>
+      <c r="K50" s="8"/>
+      <c r="L50" s="8"/>
+      <c r="M50" s="8"/>
+      <c r="N50" s="8"/>
+      <c r="O50" s="8"/>
+      <c r="P50" s="8"/>
+      <c r="Q50" s="8"/>
+      <c r="R50" s="8"/>
+      <c r="S50" s="8"/>
+      <c r="T50" s="8"/>
+      <c r="U50" s="8"/>
+      <c r="V50" s="8"/>
+      <c r="W50" s="8"/>
+      <c r="X50" s="8"/>
+      <c r="Y50" s="8"/>
+      <c r="Z50" s="8"/>
+    </row>
+    <row r="51" spans="1:26" s="9" customFormat="1" ht="21" customHeight="1">
+      <c r="A51" s="23"/>
+      <c r="B51" s="27"/>
+      <c r="C51" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E51" s="10"/>
+      <c r="F51" s="21"/>
+      <c r="G51" s="18"/>
+      <c r="H51" s="11"/>
+      <c r="I51" s="8"/>
+      <c r="J51" s="8"/>
+      <c r="K51" s="8"/>
+      <c r="L51" s="8"/>
+      <c r="M51" s="8"/>
+      <c r="N51" s="8"/>
+      <c r="O51" s="8"/>
+      <c r="P51" s="8"/>
+      <c r="Q51" s="8"/>
+      <c r="R51" s="8"/>
+      <c r="S51" s="8"/>
+      <c r="T51" s="8"/>
+      <c r="U51" s="8"/>
+      <c r="V51" s="8"/>
+      <c r="W51" s="8"/>
+      <c r="X51" s="8"/>
+      <c r="Y51" s="8"/>
+      <c r="Z51" s="8"/>
+    </row>
+    <row r="52" spans="1:26" s="9" customFormat="1" ht="21" customHeight="1">
+      <c r="A52" s="23"/>
+      <c r="B52" s="27"/>
+      <c r="C52" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E52" s="10"/>
+      <c r="F52" s="21"/>
+      <c r="G52" s="18"/>
+      <c r="H52" s="11"/>
+      <c r="I52" s="8"/>
+      <c r="J52" s="8"/>
+      <c r="K52" s="8"/>
+      <c r="L52" s="8"/>
+      <c r="M52" s="8"/>
+      <c r="N52" s="8"/>
+      <c r="O52" s="8"/>
+      <c r="P52" s="8"/>
+      <c r="Q52" s="8"/>
+      <c r="R52" s="8"/>
+      <c r="S52" s="8"/>
+      <c r="T52" s="8"/>
+      <c r="U52" s="8"/>
+      <c r="V52" s="8"/>
+      <c r="W52" s="8"/>
+      <c r="X52" s="8"/>
+      <c r="Y52" s="8"/>
+      <c r="Z52" s="8"/>
+    </row>
+    <row r="53" spans="1:26" s="43" customFormat="1" ht="3.75" customHeight="1">
+      <c r="A53" s="37"/>
+      <c r="B53" s="38"/>
+      <c r="C53" s="39"/>
+      <c r="D53" s="40"/>
+      <c r="E53" s="41"/>
+      <c r="F53" s="44"/>
+      <c r="G53" s="37"/>
+      <c r="H53" s="45"/>
+      <c r="I53" s="42"/>
+      <c r="J53" s="42"/>
+      <c r="K53" s="42"/>
+      <c r="L53" s="42"/>
+      <c r="M53" s="42"/>
+      <c r="N53" s="42"/>
+      <c r="O53" s="42"/>
+      <c r="P53" s="42"/>
+      <c r="Q53" s="42"/>
+      <c r="R53" s="42"/>
+      <c r="S53" s="42"/>
+      <c r="T53" s="42"/>
+      <c r="U53" s="42"/>
+      <c r="V53" s="42"/>
+      <c r="W53" s="42"/>
+      <c r="X53" s="42"/>
+      <c r="Y53" s="42"/>
+      <c r="Z53" s="42"/>
+    </row>
+    <row r="54" spans="1:26" s="9" customFormat="1" ht="21" customHeight="1">
+      <c r="A54" s="23">
+        <v>6</v>
+      </c>
+      <c r="B54" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D54" s="24"/>
+      <c r="E54" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="F54" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="G54" s="18"/>
+      <c r="H54" s="11"/>
+      <c r="I54" s="8"/>
+      <c r="J54" s="8"/>
+      <c r="K54" s="8"/>
+      <c r="L54" s="8"/>
+      <c r="M54" s="8"/>
+      <c r="N54" s="8"/>
+      <c r="O54" s="8"/>
+      <c r="P54" s="8"/>
+      <c r="Q54" s="8"/>
+      <c r="R54" s="8"/>
+      <c r="S54" s="8"/>
+      <c r="T54" s="8"/>
+      <c r="U54" s="8"/>
+      <c r="V54" s="8"/>
+      <c r="W54" s="8"/>
+      <c r="X54" s="8"/>
+      <c r="Y54" s="8"/>
+      <c r="Z54" s="8"/>
+    </row>
+    <row r="55" spans="1:26" s="9" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A55" s="23"/>
+      <c r="B55" s="27"/>
+      <c r="C55" s="34"/>
+      <c r="D55" s="24"/>
+      <c r="E55" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="F55" s="21"/>
+      <c r="G55" s="18"/>
+      <c r="H55" s="11"/>
+      <c r="I55" s="8"/>
+      <c r="J55" s="8"/>
+      <c r="K55" s="8"/>
+      <c r="L55" s="8"/>
+      <c r="M55" s="8"/>
+      <c r="N55" s="8"/>
+      <c r="O55" s="8"/>
+      <c r="P55" s="8"/>
+      <c r="Q55" s="8"/>
+      <c r="R55" s="8"/>
+      <c r="S55" s="8"/>
+      <c r="T55" s="8"/>
+      <c r="U55" s="8"/>
+      <c r="V55" s="8"/>
+      <c r="W55" s="8"/>
+      <c r="X55" s="8"/>
+      <c r="Y55" s="8"/>
+      <c r="Z55" s="8"/>
+    </row>
+    <row r="56" spans="1:26" s="9" customFormat="1" ht="21" customHeight="1">
+      <c r="A56" s="23"/>
+      <c r="B56" s="27"/>
+      <c r="C56" s="34"/>
+      <c r="D56" s="24"/>
+      <c r="E56" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="F56" s="21"/>
+      <c r="G56" s="18"/>
+      <c r="H56" s="11"/>
+      <c r="I56" s="8"/>
+      <c r="J56" s="8"/>
+      <c r="K56" s="8"/>
+      <c r="L56" s="8"/>
+      <c r="M56" s="8"/>
+      <c r="N56" s="8"/>
+      <c r="O56" s="8"/>
+      <c r="P56" s="8"/>
+      <c r="Q56" s="8"/>
+      <c r="R56" s="8"/>
+      <c r="S56" s="8"/>
+      <c r="T56" s="8"/>
+      <c r="U56" s="8"/>
+      <c r="V56" s="8"/>
+      <c r="W56" s="8"/>
+      <c r="X56" s="8"/>
+      <c r="Y56" s="8"/>
+      <c r="Z56" s="8"/>
+    </row>
+    <row r="57" spans="1:26" s="43" customFormat="1" ht="3.75" customHeight="1">
+      <c r="A57" s="37"/>
+      <c r="B57" s="38"/>
+      <c r="C57" s="39"/>
+      <c r="D57" s="40"/>
+      <c r="E57" s="41"/>
+      <c r="F57" s="44"/>
+      <c r="G57" s="37"/>
+      <c r="H57" s="45"/>
+      <c r="I57" s="42"/>
+      <c r="J57" s="42"/>
+      <c r="K57" s="42"/>
+      <c r="L57" s="42"/>
+      <c r="M57" s="42"/>
+      <c r="N57" s="42"/>
+      <c r="O57" s="42"/>
+      <c r="P57" s="42"/>
+      <c r="Q57" s="42"/>
+      <c r="R57" s="42"/>
+      <c r="S57" s="42"/>
+      <c r="T57" s="42"/>
+      <c r="U57" s="42"/>
+      <c r="V57" s="42"/>
+      <c r="W57" s="42"/>
+      <c r="X57" s="42"/>
+      <c r="Y57" s="42"/>
+      <c r="Z57" s="42"/>
+    </row>
+    <row r="58" spans="1:26" s="9" customFormat="1" ht="33" customHeight="1">
+      <c r="A58" s="18">
+        <v>7</v>
+      </c>
+      <c r="B58" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C58" s="3"/>
+      <c r="D58" s="19"/>
+      <c r="E58" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="F58" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="G58" s="18"/>
+      <c r="H58" s="11"/>
+      <c r="I58" s="8"/>
+      <c r="J58" s="8"/>
+      <c r="K58" s="8"/>
+      <c r="L58" s="8"/>
+      <c r="M58" s="8"/>
+      <c r="N58" s="8"/>
+      <c r="O58" s="8"/>
+      <c r="P58" s="8"/>
+      <c r="Q58" s="8"/>
+      <c r="R58" s="8"/>
+      <c r="S58" s="8"/>
+      <c r="T58" s="8"/>
+      <c r="U58" s="8"/>
+      <c r="V58" s="8"/>
+      <c r="W58" s="8"/>
+      <c r="X58" s="8"/>
+      <c r="Y58" s="8"/>
+      <c r="Z58" s="8"/>
+    </row>
+    <row r="59" spans="1:26" s="43" customFormat="1" ht="3.75" customHeight="1">
+      <c r="A59" s="37"/>
+      <c r="B59" s="38"/>
+      <c r="C59" s="39"/>
+      <c r="D59" s="40"/>
+      <c r="E59" s="41"/>
+      <c r="F59" s="44"/>
+      <c r="G59" s="37"/>
+      <c r="H59" s="45"/>
+      <c r="I59" s="42"/>
+      <c r="J59" s="42"/>
+      <c r="K59" s="42"/>
+      <c r="L59" s="42"/>
+      <c r="M59" s="42"/>
+      <c r="N59" s="42"/>
+      <c r="O59" s="42"/>
+      <c r="P59" s="42"/>
+      <c r="Q59" s="42"/>
+      <c r="R59" s="42"/>
+      <c r="S59" s="42"/>
+      <c r="T59" s="42"/>
+      <c r="U59" s="42"/>
+      <c r="V59" s="42"/>
+      <c r="W59" s="42"/>
+      <c r="X59" s="42"/>
+      <c r="Y59" s="42"/>
+      <c r="Z59" s="42"/>
+    </row>
+    <row r="60" spans="1:26" s="9" customFormat="1" ht="33.75" customHeight="1">
+      <c r="A60" s="18">
+        <v>8</v>
+      </c>
+      <c r="B60" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D60" s="19"/>
+      <c r="E60" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="F60" s="21"/>
+      <c r="G60" s="18"/>
+      <c r="H60" s="11"/>
+      <c r="I60" s="8"/>
+      <c r="J60" s="8"/>
+      <c r="K60" s="8"/>
+      <c r="L60" s="8"/>
+      <c r="M60" s="8"/>
+      <c r="N60" s="8"/>
+      <c r="O60" s="8"/>
+      <c r="P60" s="8"/>
+      <c r="Q60" s="8"/>
+      <c r="R60" s="8"/>
+      <c r="S60" s="8"/>
+      <c r="T60" s="8"/>
+      <c r="U60" s="8"/>
+      <c r="V60" s="8"/>
+      <c r="W60" s="8"/>
+      <c r="X60" s="8"/>
+      <c r="Y60" s="8"/>
+      <c r="Z60" s="8"/>
+    </row>
+    <row r="61" spans="1:26" s="9" customFormat="1" ht="33.75" customHeight="1">
+      <c r="A61" s="18"/>
+      <c r="B61" s="17"/>
+      <c r="C61" s="3"/>
+      <c r="D61" s="19"/>
+      <c r="E61" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="F61" s="21"/>
+      <c r="G61" s="18"/>
+      <c r="H61" s="11"/>
+      <c r="I61" s="8"/>
+      <c r="J61" s="8"/>
+      <c r="K61" s="8"/>
+      <c r="L61" s="8"/>
+      <c r="M61" s="8"/>
+      <c r="N61" s="8"/>
+      <c r="O61" s="8"/>
+      <c r="P61" s="8"/>
+      <c r="Q61" s="8"/>
+      <c r="R61" s="8"/>
+      <c r="S61" s="8"/>
+      <c r="T61" s="8"/>
+      <c r="U61" s="8"/>
+      <c r="V61" s="8"/>
+      <c r="W61" s="8"/>
+      <c r="X61" s="8"/>
+      <c r="Y61" s="8"/>
+      <c r="Z61" s="8"/>
+    </row>
+    <row r="62" spans="1:26" s="9" customFormat="1" ht="33.75" customHeight="1">
+      <c r="A62" s="18"/>
+      <c r="B62" s="17"/>
+      <c r="C62" s="3"/>
+      <c r="D62" s="19"/>
+      <c r="E62" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="F62" s="21"/>
+      <c r="G62" s="18"/>
+      <c r="H62" s="11"/>
+      <c r="I62" s="8"/>
+      <c r="J62" s="8"/>
+      <c r="K62" s="8"/>
+      <c r="L62" s="8"/>
+      <c r="M62" s="8"/>
+      <c r="N62" s="8"/>
+      <c r="O62" s="8"/>
+      <c r="P62" s="8"/>
+      <c r="Q62" s="8"/>
+      <c r="R62" s="8"/>
+      <c r="S62" s="8"/>
+      <c r="T62" s="8"/>
+      <c r="U62" s="8"/>
+      <c r="V62" s="8"/>
+      <c r="W62" s="8"/>
+      <c r="X62" s="8"/>
+      <c r="Y62" s="8"/>
+      <c r="Z62" s="8"/>
+    </row>
+    <row r="63" spans="1:26" s="9" customFormat="1" ht="33.75" customHeight="1">
+      <c r="A63" s="18"/>
+      <c r="B63" s="17"/>
+      <c r="C63" s="3"/>
+      <c r="D63" s="19"/>
+      <c r="E63" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="F63" s="21"/>
+      <c r="G63" s="18"/>
+      <c r="H63" s="11"/>
+      <c r="I63" s="8"/>
+      <c r="J63" s="8"/>
+      <c r="K63" s="8"/>
+      <c r="L63" s="8"/>
+      <c r="M63" s="8"/>
+      <c r="N63" s="8"/>
+      <c r="O63" s="8"/>
+      <c r="P63" s="8"/>
+      <c r="Q63" s="8"/>
+      <c r="R63" s="8"/>
+      <c r="S63" s="8"/>
+      <c r="T63" s="8"/>
+      <c r="U63" s="8"/>
+      <c r="V63" s="8"/>
+      <c r="W63" s="8"/>
+      <c r="X63" s="8"/>
+      <c r="Y63" s="8"/>
+      <c r="Z63" s="8"/>
+    </row>
+    <row r="64" spans="1:26" s="43" customFormat="1" ht="3.75" customHeight="1">
+      <c r="A64" s="37"/>
+      <c r="B64" s="38"/>
+      <c r="C64" s="39"/>
+      <c r="D64" s="40"/>
+      <c r="E64" s="41"/>
+      <c r="F64" s="44"/>
+      <c r="G64" s="37"/>
+      <c r="H64" s="45"/>
+      <c r="I64" s="42"/>
+      <c r="J64" s="42"/>
+      <c r="K64" s="42"/>
+      <c r="L64" s="42"/>
+      <c r="M64" s="42"/>
+      <c r="N64" s="42"/>
+      <c r="O64" s="42"/>
+      <c r="P64" s="42"/>
+      <c r="Q64" s="42"/>
+      <c r="R64" s="42"/>
+      <c r="S64" s="42"/>
+      <c r="T64" s="42"/>
+      <c r="U64" s="42"/>
+      <c r="V64" s="42"/>
+      <c r="W64" s="42"/>
+      <c r="X64" s="42"/>
+      <c r="Y64" s="42"/>
+      <c r="Z64" s="42"/>
+    </row>
+    <row r="65" spans="1:26" s="9" customFormat="1" ht="33.75" customHeight="1">
+      <c r="A65" s="18">
+        <v>9</v>
+      </c>
+      <c r="B65" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C65" s="3"/>
+      <c r="D65" s="19"/>
+      <c r="E65" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="F65" s="21"/>
+      <c r="G65" s="18"/>
+      <c r="H65" s="11"/>
+      <c r="I65" s="8"/>
+      <c r="J65" s="8"/>
+      <c r="K65" s="8"/>
+      <c r="L65" s="8"/>
+      <c r="M65" s="8"/>
+      <c r="N65" s="8"/>
+      <c r="O65" s="8"/>
+      <c r="P65" s="8"/>
+      <c r="Q65" s="8"/>
+      <c r="R65" s="8"/>
+      <c r="S65" s="8"/>
+      <c r="T65" s="8"/>
+      <c r="U65" s="8"/>
+      <c r="V65" s="8"/>
+      <c r="W65" s="8"/>
+      <c r="X65" s="8"/>
+      <c r="Y65" s="8"/>
+      <c r="Z65" s="8"/>
+    </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="D29:D31"/>
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="A8:A15"/>
-    <mergeCell ref="D8:D15"/>
-    <mergeCell ref="F8:F15"/>
-    <mergeCell ref="C12:C15"/>
-    <mergeCell ref="A21:A25"/>
-    <mergeCell ref="B21:B25"/>
-    <mergeCell ref="D21:D25"/>
-    <mergeCell ref="B16:B20"/>
-    <mergeCell ref="A16:A20"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="E23:E25"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="B54:B56"/>
+    <mergeCell ref="A54:A56"/>
+    <mergeCell ref="D54:D56"/>
+    <mergeCell ref="A50:A52"/>
+    <mergeCell ref="B50:B52"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="A9:A27"/>
+    <mergeCell ref="D9:D27"/>
+    <mergeCell ref="F9:F27"/>
+    <mergeCell ref="C13:C27"/>
+    <mergeCell ref="A44:A48"/>
+    <mergeCell ref="B44:B48"/>
+    <mergeCell ref="D44:D48"/>
+    <mergeCell ref="B37:B41"/>
+    <mergeCell ref="A37:A41"/>
+    <mergeCell ref="C47:C48"/>
+    <mergeCell ref="E46:E48"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="H9:H10"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B8:B15"/>
+    <mergeCell ref="B9:B27"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="F6:F7"/>

</xml_diff>

<commit_message>
Design Document column has been updated
</commit_message>
<xml_diff>
--- a/Lhub_RTM_v1.xlsx
+++ b/Lhub_RTM_v1.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\Project management\Learning-hub project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mazmy\Documents\GitHub\Learning-hub\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="103">
   <si>
     <t>Requirements Traceability Matrix</t>
   </si>
@@ -240,18 +240,6 @@
     <t>Ragab</t>
   </si>
   <si>
-    <t>Lhub_SDD_4.1.2</t>
-  </si>
-  <si>
-    <t>Lhub_SDD_4.1.4</t>
-  </si>
-  <si>
-    <t>Lhub_SDD_4.1.3</t>
-  </si>
-  <si>
-    <t>Lhub_SDD_4.1.1</t>
-  </si>
-  <si>
     <t>Lhub_SRS_2.4.1.6</t>
   </si>
   <si>
@@ -331,6 +319,30 @@
   </si>
   <si>
     <t>Aya</t>
+  </si>
+  <si>
+    <t>Lhub_SDD_4.1.1
+Lhub_SDD_5.2.1
+Lhub_SDD_5.2.2</t>
+  </si>
+  <si>
+    <t>Lhub_SDD_4.1.3
+Lhub_SDD_5.2.9</t>
+  </si>
+  <si>
+    <t>Lhub_SDD_4.1.4
+Lhub_SDD_5.2.3</t>
+  </si>
+  <si>
+    <t>Lhub_SDD_4.1.2
+Lhub_SDD_5.2.4</t>
+  </si>
+  <si>
+    <t>Lhub_SDD_5.2.4</t>
+  </si>
+  <si>
+    <t>Lhub_SDD_5.2.5
+Lhub_SDD_5.2.6</t>
   </si>
 </sst>
 </file>
@@ -506,7 +518,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -529,13 +541,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -597,21 +646,6 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -624,19 +658,12 @@
     <xf numFmtId="0" fontId="16" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -661,6 +688,67 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -989,21 +1077,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" style="12" customWidth="1"/>
-    <col min="2" max="2" width="30.42578125" style="12" customWidth="1"/>
-    <col min="3" max="3" width="48.140625" style="12" customWidth="1"/>
-    <col min="4" max="4" width="23.28515625" style="12" customWidth="1"/>
-    <col min="5" max="5" width="35.85546875" style="12" customWidth="1"/>
+    <col min="1" max="1" width="23.26953125" style="12" customWidth="1"/>
+    <col min="2" max="2" width="30.453125" style="12" customWidth="1"/>
+    <col min="3" max="3" width="48.1796875" style="12" customWidth="1"/>
+    <col min="4" max="4" width="23.26953125" style="12" customWidth="1"/>
+    <col min="5" max="5" width="35.81640625" style="12" customWidth="1"/>
     <col min="6" max="6" width="38" style="22" customWidth="1"/>
-    <col min="7" max="7" width="37.5703125" style="12" customWidth="1"/>
-    <col min="8" max="8" width="44.5703125" style="12" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="12"/>
+    <col min="7" max="7" width="37.54296875" style="12" customWidth="1"/>
+    <col min="8" max="8" width="44.54296875" style="12" customWidth="1"/>
+    <col min="9" max="16384" width="9.1796875" style="12"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="4" customFormat="1" ht="30" customHeight="1">
@@ -1016,23 +1104,23 @@
       <c r="A2" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="28" t="s">
+      <c r="C2" s="44"/>
+      <c r="D2" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="F2" s="28" t="s">
+      <c r="F2" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="G2" s="28" t="s">
+      <c r="G2" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="H2" s="28" t="s">
+      <c r="H2" s="23" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1040,11 +1128,11 @@
       <c r="A3" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="29" t="s">
+      <c r="C3" s="44"/>
+      <c r="D3" s="24" t="s">
         <v>66</v>
       </c>
       <c r="E3" s="14">
@@ -1064,23 +1152,23 @@
       <c r="A4" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="26">
+      <c r="B4" s="45">
         <v>43470</v>
       </c>
-      <c r="C4" s="26"/>
-      <c r="D4" s="30"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="25"/>
       <c r="E4" s="14">
         <v>43592</v>
       </c>
-      <c r="F4" s="31"/>
+      <c r="F4" s="26"/>
       <c r="G4" s="15" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="H4" s="15" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" s="7" customFormat="1" ht="33.75" customHeight="1">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" s="7" customFormat="1" ht="25">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -1125,22 +1213,22 @@
       <c r="Z5" s="6"/>
     </row>
     <row r="6" spans="1:26" s="9" customFormat="1" ht="24.75" customHeight="1">
-      <c r="A6" s="23">
+      <c r="A6" s="39">
         <v>1</v>
       </c>
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="38" t="s">
         <v>32</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="24"/>
+      <c r="D6" s="40"/>
       <c r="E6" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="32"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="46"/>
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
       <c r="K6" s="8"/>
@@ -1160,19 +1248,19 @@
       <c r="Y6" s="8"/>
       <c r="Z6" s="8"/>
     </row>
-    <row r="7" spans="1:26" s="9" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A7" s="23"/>
-      <c r="B7" s="27"/>
+    <row r="7" spans="1:26" s="9" customFormat="1">
+      <c r="A7" s="39"/>
+      <c r="B7" s="38"/>
       <c r="C7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="24"/>
+      <c r="D7" s="40"/>
       <c r="E7" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="32"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="46"/>
+      <c r="H7" s="46"/>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
       <c r="K7" s="8"/>
@@ -1192,53 +1280,53 @@
       <c r="Y7" s="8"/>
       <c r="Z7" s="8"/>
     </row>
-    <row r="8" spans="1:26" s="43" customFormat="1" ht="3.75" customHeight="1">
-      <c r="A8" s="37"/>
-      <c r="B8" s="38"/>
-      <c r="C8" s="39"/>
-      <c r="D8" s="40"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
-      <c r="G8" s="41"/>
-      <c r="H8" s="41"/>
-      <c r="I8" s="42"/>
-      <c r="J8" s="42"/>
-      <c r="K8" s="42"/>
-      <c r="L8" s="42"/>
-      <c r="M8" s="42"/>
-      <c r="N8" s="42"/>
-      <c r="O8" s="42"/>
-      <c r="P8" s="42"/>
-      <c r="Q8" s="42"/>
-      <c r="R8" s="42"/>
-      <c r="S8" s="42"/>
-      <c r="T8" s="42"/>
-      <c r="U8" s="42"/>
-      <c r="V8" s="42"/>
-      <c r="W8" s="42"/>
-      <c r="X8" s="42"/>
-      <c r="Y8" s="42"/>
-      <c r="Z8" s="42"/>
+    <row r="8" spans="1:26" s="35" customFormat="1" ht="3.75" customHeight="1">
+      <c r="A8" s="29"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="34"/>
+      <c r="J8" s="34"/>
+      <c r="K8" s="34"/>
+      <c r="L8" s="34"/>
+      <c r="M8" s="34"/>
+      <c r="N8" s="34"/>
+      <c r="O8" s="34"/>
+      <c r="P8" s="34"/>
+      <c r="Q8" s="34"/>
+      <c r="R8" s="34"/>
+      <c r="S8" s="34"/>
+      <c r="T8" s="34"/>
+      <c r="U8" s="34"/>
+      <c r="V8" s="34"/>
+      <c r="W8" s="34"/>
+      <c r="X8" s="34"/>
+      <c r="Y8" s="34"/>
+      <c r="Z8" s="34"/>
     </row>
     <row r="9" spans="1:26" s="9" customFormat="1" ht="18" customHeight="1">
-      <c r="A9" s="23">
+      <c r="A9" s="39">
         <v>2</v>
       </c>
-      <c r="B9" s="27" t="s">
+      <c r="B9" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="24"/>
+      <c r="D9" s="40"/>
       <c r="E9" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="F9" s="33" t="s">
-        <v>73</v>
-      </c>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
+      <c r="F9" s="47" t="s">
+        <v>97</v>
+      </c>
+      <c r="G9" s="39"/>
+      <c r="H9" s="39"/>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
@@ -1259,18 +1347,18 @@
       <c r="Z9" s="8"/>
     </row>
     <row r="10" spans="1:26" s="9" customFormat="1" ht="21" customHeight="1">
-      <c r="A10" s="23"/>
-      <c r="B10" s="27"/>
-      <c r="C10" s="3" t="s">
+      <c r="A10" s="39"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="24"/>
+      <c r="D10" s="40"/>
       <c r="E10" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="F10" s="33"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="23"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="39"/>
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
       <c r="K10" s="8"/>
@@ -1291,16 +1379,16 @@
       <c r="Z10" s="8"/>
     </row>
     <row r="11" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A11" s="23"/>
-      <c r="B11" s="27"/>
-      <c r="C11" s="3" t="s">
+      <c r="A11" s="39"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="24"/>
+      <c r="D11" s="40"/>
       <c r="E11" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="F11" s="33"/>
+      <c r="F11" s="42"/>
       <c r="G11" s="18"/>
       <c r="H11" s="11"/>
       <c r="I11" s="8"/>
@@ -1323,16 +1411,16 @@
       <c r="Z11" s="8"/>
     </row>
     <row r="12" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A12" s="23"/>
-      <c r="B12" s="27"/>
-      <c r="C12" s="3" t="s">
+      <c r="A12" s="39"/>
+      <c r="B12" s="38"/>
+      <c r="C12" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="D12" s="24"/>
+      <c r="D12" s="40"/>
       <c r="E12" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="F12" s="33"/>
+      <c r="F12" s="42"/>
       <c r="G12" s="18"/>
       <c r="H12" s="11"/>
       <c r="I12" s="8"/>
@@ -1355,14 +1443,14 @@
       <c r="Z12" s="8"/>
     </row>
     <row r="13" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A13" s="23"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="34"/>
-      <c r="D13" s="24"/>
+      <c r="A13" s="39"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="58"/>
+      <c r="D13" s="40"/>
       <c r="E13" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="F13" s="33"/>
+      <c r="F13" s="42"/>
       <c r="G13" s="18"/>
       <c r="H13" s="11"/>
       <c r="I13" s="8"/>
@@ -1385,14 +1473,14 @@
       <c r="Z13" s="8"/>
     </row>
     <row r="14" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A14" s="23"/>
-      <c r="B14" s="27"/>
-      <c r="C14" s="34"/>
-      <c r="D14" s="24"/>
+      <c r="A14" s="39"/>
+      <c r="B14" s="38"/>
+      <c r="C14" s="58"/>
+      <c r="D14" s="40"/>
       <c r="E14" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="F14" s="33"/>
+        <v>70</v>
+      </c>
+      <c r="F14" s="42"/>
       <c r="G14" s="18"/>
       <c r="H14" s="11"/>
       <c r="I14" s="8"/>
@@ -1415,14 +1503,14 @@
       <c r="Z14" s="8"/>
     </row>
     <row r="15" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A15" s="23"/>
-      <c r="B15" s="27"/>
-      <c r="C15" s="34"/>
-      <c r="D15" s="24"/>
+      <c r="A15" s="39"/>
+      <c r="B15" s="38"/>
+      <c r="C15" s="58"/>
+      <c r="D15" s="40"/>
       <c r="E15" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="F15" s="33"/>
+        <v>71</v>
+      </c>
+      <c r="F15" s="42"/>
       <c r="G15" s="18"/>
       <c r="H15" s="11"/>
       <c r="I15" s="8"/>
@@ -1445,14 +1533,14 @@
       <c r="Z15" s="8"/>
     </row>
     <row r="16" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A16" s="23"/>
-      <c r="B16" s="27"/>
-      <c r="C16" s="34"/>
-      <c r="D16" s="24"/>
+      <c r="A16" s="39"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="58"/>
+      <c r="D16" s="40"/>
       <c r="E16" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="F16" s="33"/>
+        <v>72</v>
+      </c>
+      <c r="F16" s="42"/>
       <c r="G16" s="18"/>
       <c r="H16" s="11"/>
       <c r="I16" s="8"/>
@@ -1475,14 +1563,14 @@
       <c r="Z16" s="8"/>
     </row>
     <row r="17" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A17" s="23"/>
-      <c r="B17" s="27"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="24"/>
+      <c r="A17" s="39"/>
+      <c r="B17" s="38"/>
+      <c r="C17" s="58"/>
+      <c r="D17" s="40"/>
       <c r="E17" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="F17" s="33"/>
+        <v>73</v>
+      </c>
+      <c r="F17" s="42"/>
       <c r="G17" s="18"/>
       <c r="H17" s="11"/>
       <c r="I17" s="8"/>
@@ -1505,14 +1593,14 @@
       <c r="Z17" s="8"/>
     </row>
     <row r="18" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A18" s="23"/>
-      <c r="B18" s="27"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="24"/>
+      <c r="A18" s="39"/>
+      <c r="B18" s="38"/>
+      <c r="C18" s="58"/>
+      <c r="D18" s="40"/>
       <c r="E18" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="F18" s="33"/>
+        <v>74</v>
+      </c>
+      <c r="F18" s="42"/>
       <c r="G18" s="18"/>
       <c r="H18" s="11"/>
       <c r="I18" s="8"/>
@@ -1535,14 +1623,14 @@
       <c r="Z18" s="8"/>
     </row>
     <row r="19" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A19" s="23"/>
-      <c r="B19" s="27"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="24"/>
+      <c r="A19" s="39"/>
+      <c r="B19" s="38"/>
+      <c r="C19" s="58"/>
+      <c r="D19" s="40"/>
       <c r="E19" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="F19" s="33"/>
+        <v>75</v>
+      </c>
+      <c r="F19" s="42"/>
       <c r="G19" s="18"/>
       <c r="H19" s="11"/>
       <c r="I19" s="8"/>
@@ -1565,14 +1653,14 @@
       <c r="Z19" s="8"/>
     </row>
     <row r="20" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A20" s="23"/>
-      <c r="B20" s="27"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="24"/>
+      <c r="A20" s="39"/>
+      <c r="B20" s="38"/>
+      <c r="C20" s="58"/>
+      <c r="D20" s="40"/>
       <c r="E20" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="F20" s="33"/>
+        <v>76</v>
+      </c>
+      <c r="F20" s="42"/>
       <c r="G20" s="18"/>
       <c r="H20" s="11"/>
       <c r="I20" s="8"/>
@@ -1595,14 +1683,14 @@
       <c r="Z20" s="8"/>
     </row>
     <row r="21" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A21" s="23"/>
-      <c r="B21" s="27"/>
-      <c r="C21" s="34"/>
-      <c r="D21" s="24"/>
+      <c r="A21" s="39"/>
+      <c r="B21" s="38"/>
+      <c r="C21" s="58"/>
+      <c r="D21" s="40"/>
       <c r="E21" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="F21" s="33"/>
+        <v>77</v>
+      </c>
+      <c r="F21" s="42"/>
       <c r="G21" s="18"/>
       <c r="H21" s="11"/>
       <c r="I21" s="8"/>
@@ -1625,14 +1713,14 @@
       <c r="Z21" s="8"/>
     </row>
     <row r="22" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A22" s="23"/>
-      <c r="B22" s="27"/>
-      <c r="C22" s="34"/>
-      <c r="D22" s="24"/>
+      <c r="A22" s="39"/>
+      <c r="B22" s="38"/>
+      <c r="C22" s="58"/>
+      <c r="D22" s="40"/>
       <c r="E22" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="F22" s="33"/>
+        <v>78</v>
+      </c>
+      <c r="F22" s="42"/>
       <c r="G22" s="18"/>
       <c r="H22" s="11"/>
       <c r="I22" s="8"/>
@@ -1655,14 +1743,14 @@
       <c r="Z22" s="8"/>
     </row>
     <row r="23" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A23" s="23"/>
-      <c r="B23" s="27"/>
-      <c r="C23" s="34"/>
-      <c r="D23" s="24"/>
+      <c r="A23" s="39"/>
+      <c r="B23" s="38"/>
+      <c r="C23" s="58"/>
+      <c r="D23" s="40"/>
       <c r="E23" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="F23" s="33"/>
+      <c r="F23" s="42"/>
       <c r="G23" s="18"/>
       <c r="H23" s="11"/>
       <c r="I23" s="8"/>
@@ -1685,14 +1773,14 @@
       <c r="Z23" s="8"/>
     </row>
     <row r="24" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A24" s="23"/>
-      <c r="B24" s="27"/>
-      <c r="C24" s="34"/>
-      <c r="D24" s="24"/>
+      <c r="A24" s="39"/>
+      <c r="B24" s="38"/>
+      <c r="C24" s="58"/>
+      <c r="D24" s="40"/>
       <c r="E24" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="F24" s="33"/>
+      <c r="F24" s="42"/>
       <c r="G24" s="18"/>
       <c r="H24" s="11"/>
       <c r="I24" s="8"/>
@@ -1715,14 +1803,14 @@
       <c r="Z24" s="8"/>
     </row>
     <row r="25" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A25" s="23"/>
-      <c r="B25" s="27"/>
-      <c r="C25" s="34"/>
-      <c r="D25" s="24"/>
+      <c r="A25" s="39"/>
+      <c r="B25" s="38"/>
+      <c r="C25" s="58"/>
+      <c r="D25" s="40"/>
       <c r="E25" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="F25" s="33"/>
+      <c r="F25" s="42"/>
       <c r="G25" s="18"/>
       <c r="H25" s="11"/>
       <c r="I25" s="8"/>
@@ -1745,14 +1833,14 @@
       <c r="Z25" s="8"/>
     </row>
     <row r="26" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A26" s="23"/>
-      <c r="B26" s="27"/>
-      <c r="C26" s="34"/>
-      <c r="D26" s="24"/>
+      <c r="A26" s="39"/>
+      <c r="B26" s="38"/>
+      <c r="C26" s="58"/>
+      <c r="D26" s="40"/>
       <c r="E26" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="F26" s="33"/>
+        <v>79</v>
+      </c>
+      <c r="F26" s="42"/>
       <c r="G26" s="18"/>
       <c r="H26" s="11"/>
       <c r="I26" s="8"/>
@@ -1775,14 +1863,14 @@
       <c r="Z26" s="8"/>
     </row>
     <row r="27" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A27" s="23"/>
-      <c r="B27" s="27"/>
-      <c r="C27" s="34"/>
-      <c r="D27" s="24"/>
+      <c r="A27" s="39"/>
+      <c r="B27" s="38"/>
+      <c r="C27" s="58"/>
+      <c r="D27" s="40"/>
       <c r="E27" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="F27" s="33"/>
+        <v>80</v>
+      </c>
+      <c r="F27" s="42"/>
       <c r="G27" s="18"/>
       <c r="H27" s="11"/>
       <c r="I27" s="8"/>
@@ -1807,10 +1895,10 @@
     <row r="28" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
       <c r="A28" s="18"/>
       <c r="B28" s="17"/>
-      <c r="C28" s="3"/>
+      <c r="C28" s="27"/>
       <c r="D28" s="19"/>
       <c r="E28" s="10" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="F28" s="21"/>
       <c r="G28" s="18"/>
@@ -1837,10 +1925,10 @@
     <row r="29" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
       <c r="A29" s="18"/>
       <c r="B29" s="17"/>
-      <c r="C29" s="3"/>
+      <c r="C29" s="27"/>
       <c r="D29" s="19"/>
       <c r="E29" s="10" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F29" s="21"/>
       <c r="G29" s="18"/>
@@ -1867,10 +1955,10 @@
     <row r="30" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
       <c r="A30" s="18"/>
       <c r="B30" s="17"/>
-      <c r="C30" s="3"/>
+      <c r="C30" s="27"/>
       <c r="D30" s="19"/>
       <c r="E30" s="10" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F30" s="21"/>
       <c r="G30" s="18"/>
@@ -1897,10 +1985,10 @@
     <row r="31" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
       <c r="A31" s="18"/>
       <c r="B31" s="17"/>
-      <c r="C31" s="3"/>
+      <c r="C31" s="27"/>
       <c r="D31" s="19"/>
       <c r="E31" s="10" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F31" s="21"/>
       <c r="G31" s="18"/>
@@ -1927,10 +2015,10 @@
     <row r="32" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
       <c r="A32" s="18"/>
       <c r="B32" s="17"/>
-      <c r="C32" s="3"/>
+      <c r="C32" s="27"/>
       <c r="D32" s="19"/>
       <c r="E32" s="10" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="F32" s="21"/>
       <c r="G32" s="18"/>
@@ -1957,10 +2045,10 @@
     <row r="33" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
       <c r="A33" s="18"/>
       <c r="B33" s="17"/>
-      <c r="C33" s="3"/>
+      <c r="C33" s="27"/>
       <c r="D33" s="19"/>
       <c r="E33" s="10" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="F33" s="21"/>
       <c r="G33" s="18"/>
@@ -1987,10 +2075,10 @@
     <row r="34" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
       <c r="A34" s="18"/>
       <c r="B34" s="17"/>
-      <c r="C34" s="3"/>
+      <c r="C34" s="27"/>
       <c r="D34" s="19"/>
       <c r="E34" s="10" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="F34" s="21"/>
       <c r="G34" s="18"/>
@@ -2017,10 +2105,10 @@
     <row r="35" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
       <c r="A35" s="18"/>
       <c r="B35" s="17"/>
-      <c r="C35" s="3"/>
+      <c r="C35" s="27"/>
       <c r="D35" s="19"/>
       <c r="E35" s="10" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F35" s="21"/>
       <c r="G35" s="18"/>
@@ -2044,49 +2132,49 @@
       <c r="Y35" s="8"/>
       <c r="Z35" s="8"/>
     </row>
-    <row r="36" spans="1:26" s="43" customFormat="1" ht="3.75" customHeight="1">
-      <c r="A36" s="37"/>
-      <c r="B36" s="38"/>
-      <c r="C36" s="39"/>
-      <c r="D36" s="40"/>
-      <c r="E36" s="41"/>
-      <c r="F36" s="44"/>
-      <c r="G36" s="37"/>
-      <c r="H36" s="45"/>
-      <c r="I36" s="42"/>
-      <c r="J36" s="42"/>
-      <c r="K36" s="42"/>
-      <c r="L36" s="42"/>
-      <c r="M36" s="42"/>
-      <c r="N36" s="42"/>
-      <c r="O36" s="42"/>
-      <c r="P36" s="42"/>
-      <c r="Q36" s="42"/>
-      <c r="R36" s="42"/>
-      <c r="S36" s="42"/>
-      <c r="T36" s="42"/>
-      <c r="U36" s="42"/>
-      <c r="V36" s="42"/>
-      <c r="W36" s="42"/>
-      <c r="X36" s="42"/>
-      <c r="Y36" s="42"/>
-      <c r="Z36" s="42"/>
+    <row r="36" spans="1:26" s="35" customFormat="1" ht="3.75" customHeight="1">
+      <c r="A36" s="29"/>
+      <c r="B36" s="30"/>
+      <c r="C36" s="31"/>
+      <c r="D36" s="32"/>
+      <c r="E36" s="33"/>
+      <c r="F36" s="36"/>
+      <c r="G36" s="29"/>
+      <c r="H36" s="37"/>
+      <c r="I36" s="34"/>
+      <c r="J36" s="34"/>
+      <c r="K36" s="34"/>
+      <c r="L36" s="34"/>
+      <c r="M36" s="34"/>
+      <c r="N36" s="34"/>
+      <c r="O36" s="34"/>
+      <c r="P36" s="34"/>
+      <c r="Q36" s="34"/>
+      <c r="R36" s="34"/>
+      <c r="S36" s="34"/>
+      <c r="T36" s="34"/>
+      <c r="U36" s="34"/>
+      <c r="V36" s="34"/>
+      <c r="W36" s="34"/>
+      <c r="X36" s="34"/>
+      <c r="Y36" s="34"/>
+      <c r="Z36" s="34"/>
     </row>
     <row r="37" spans="1:26" s="9" customFormat="1" ht="27" customHeight="1">
-      <c r="A37" s="23">
+      <c r="A37" s="39">
         <v>3</v>
       </c>
-      <c r="B37" s="27" t="s">
+      <c r="B37" s="38" t="s">
         <v>34</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E37" s="35" t="s">
+      <c r="E37" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="F37" s="21" t="s">
-        <v>72</v>
+      <c r="F37" s="50" t="s">
+        <v>98</v>
       </c>
       <c r="G37" s="18"/>
       <c r="H37" s="11"/>
@@ -2110,15 +2198,15 @@
       <c r="Z37" s="8"/>
     </row>
     <row r="38" spans="1:26" s="9" customFormat="1" ht="27" customHeight="1">
-      <c r="A38" s="23"/>
-      <c r="B38" s="27"/>
+      <c r="A38" s="39"/>
+      <c r="B38" s="38"/>
       <c r="C38" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E38" s="35" t="s">
+      <c r="E38" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="F38" s="21"/>
+      <c r="F38" s="48"/>
       <c r="G38" s="18"/>
       <c r="H38" s="11"/>
       <c r="I38" s="8"/>
@@ -2141,15 +2229,15 @@
       <c r="Z38" s="8"/>
     </row>
     <row r="39" spans="1:26" s="9" customFormat="1" ht="27" customHeight="1">
-      <c r="A39" s="23"/>
-      <c r="B39" s="27"/>
+      <c r="A39" s="39"/>
+      <c r="B39" s="38"/>
       <c r="C39" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E39" s="35" t="s">
+      <c r="E39" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="F39" s="21"/>
+      <c r="F39" s="48"/>
       <c r="G39" s="18"/>
       <c r="H39" s="11"/>
       <c r="I39" s="8"/>
@@ -2172,16 +2260,16 @@
       <c r="Z39" s="8"/>
     </row>
     <row r="40" spans="1:26" s="9" customFormat="1" ht="27" customHeight="1">
-      <c r="A40" s="23"/>
-      <c r="B40" s="27"/>
+      <c r="A40" s="39"/>
+      <c r="B40" s="38"/>
       <c r="C40" s="3" t="s">
         <v>22</v>
       </c>
       <c r="D40" s="3"/>
-      <c r="E40" s="35" t="s">
+      <c r="E40" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="F40" s="21"/>
+      <c r="F40" s="48"/>
       <c r="G40" s="18"/>
       <c r="H40" s="11"/>
       <c r="I40" s="8"/>
@@ -2204,16 +2292,16 @@
       <c r="Z40" s="8"/>
     </row>
     <row r="41" spans="1:26" s="9" customFormat="1" ht="27" customHeight="1">
-      <c r="A41" s="23"/>
-      <c r="B41" s="27"/>
+      <c r="A41" s="39"/>
+      <c r="B41" s="38"/>
       <c r="C41" s="3" t="s">
         <v>23</v>
       </c>
       <c r="D41" s="3"/>
-      <c r="E41" s="35" t="s">
+      <c r="E41" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="F41" s="21"/>
+      <c r="F41" s="48"/>
       <c r="G41" s="18"/>
       <c r="H41" s="11"/>
       <c r="I41" s="8"/>
@@ -2240,10 +2328,10 @@
       <c r="B42" s="17"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
-      <c r="E42" s="35" t="s">
+      <c r="E42" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="F42" s="21"/>
+      <c r="F42" s="49"/>
       <c r="G42" s="18"/>
       <c r="H42" s="11"/>
       <c r="I42" s="8"/>
@@ -2265,50 +2353,50 @@
       <c r="Y42" s="8"/>
       <c r="Z42" s="8"/>
     </row>
-    <row r="43" spans="1:26" s="43" customFormat="1" ht="3.75" customHeight="1">
-      <c r="A43" s="37"/>
-      <c r="B43" s="38"/>
-      <c r="C43" s="39"/>
-      <c r="D43" s="40"/>
-      <c r="E43" s="41"/>
-      <c r="F43" s="44"/>
-      <c r="G43" s="37"/>
-      <c r="H43" s="45"/>
-      <c r="I43" s="42"/>
-      <c r="J43" s="42"/>
-      <c r="K43" s="42"/>
-      <c r="L43" s="42"/>
-      <c r="M43" s="42"/>
-      <c r="N43" s="42"/>
-      <c r="O43" s="42"/>
-      <c r="P43" s="42"/>
-      <c r="Q43" s="42"/>
-      <c r="R43" s="42"/>
-      <c r="S43" s="42"/>
-      <c r="T43" s="42"/>
-      <c r="U43" s="42"/>
-      <c r="V43" s="42"/>
-      <c r="W43" s="42"/>
-      <c r="X43" s="42"/>
-      <c r="Y43" s="42"/>
-      <c r="Z43" s="42"/>
+    <row r="43" spans="1:26" s="35" customFormat="1" ht="3.75" customHeight="1">
+      <c r="A43" s="29"/>
+      <c r="B43" s="30"/>
+      <c r="C43" s="31"/>
+      <c r="D43" s="32"/>
+      <c r="E43" s="33"/>
+      <c r="F43" s="36"/>
+      <c r="G43" s="29"/>
+      <c r="H43" s="37"/>
+      <c r="I43" s="34"/>
+      <c r="J43" s="34"/>
+      <c r="K43" s="34"/>
+      <c r="L43" s="34"/>
+      <c r="M43" s="34"/>
+      <c r="N43" s="34"/>
+      <c r="O43" s="34"/>
+      <c r="P43" s="34"/>
+      <c r="Q43" s="34"/>
+      <c r="R43" s="34"/>
+      <c r="S43" s="34"/>
+      <c r="T43" s="34"/>
+      <c r="U43" s="34"/>
+      <c r="V43" s="34"/>
+      <c r="W43" s="34"/>
+      <c r="X43" s="34"/>
+      <c r="Y43" s="34"/>
+      <c r="Z43" s="34"/>
     </row>
     <row r="44" spans="1:26" s="9" customFormat="1" ht="21.75" customHeight="1">
-      <c r="A44" s="23">
+      <c r="A44" s="39">
         <v>4</v>
       </c>
-      <c r="B44" s="27" t="s">
+      <c r="B44" s="38" t="s">
         <v>35</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D44" s="24"/>
+      <c r="D44" s="40"/>
       <c r="E44" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="F44" s="21" t="s">
-        <v>72</v>
+        <v>89</v>
+      </c>
+      <c r="F44" s="50" t="s">
+        <v>98</v>
       </c>
       <c r="G44" s="11"/>
       <c r="H44" s="11"/>
@@ -2332,16 +2420,16 @@
       <c r="Z44" s="8"/>
     </row>
     <row r="45" spans="1:26" s="9" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A45" s="23"/>
-      <c r="B45" s="27"/>
+      <c r="A45" s="39"/>
+      <c r="B45" s="38"/>
       <c r="C45" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D45" s="24"/>
+      <c r="D45" s="40"/>
       <c r="E45" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="F45" s="21"/>
+        <v>90</v>
+      </c>
+      <c r="F45" s="48"/>
       <c r="G45" s="11"/>
       <c r="H45" s="11"/>
       <c r="I45" s="8"/>
@@ -2364,14 +2452,14 @@
       <c r="Z45" s="8"/>
     </row>
     <row r="46" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A46" s="23"/>
-      <c r="B46" s="27"/>
+      <c r="A46" s="39"/>
+      <c r="B46" s="38"/>
       <c r="C46" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D46" s="24"/>
-      <c r="E46" s="36"/>
-      <c r="F46" s="21"/>
+      <c r="D46" s="40"/>
+      <c r="E46" s="43"/>
+      <c r="F46" s="48"/>
       <c r="G46" s="11"/>
       <c r="H46" s="11"/>
       <c r="I46" s="8"/>
@@ -2394,12 +2482,12 @@
       <c r="Z46" s="8"/>
     </row>
     <row r="47" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A47" s="23"/>
-      <c r="B47" s="27"/>
-      <c r="C47" s="34"/>
-      <c r="D47" s="24"/>
-      <c r="E47" s="36"/>
-      <c r="F47" s="21"/>
+      <c r="A47" s="39"/>
+      <c r="B47" s="38"/>
+      <c r="C47" s="41"/>
+      <c r="D47" s="40"/>
+      <c r="E47" s="43"/>
+      <c r="F47" s="48"/>
       <c r="G47" s="11"/>
       <c r="H47" s="11"/>
       <c r="I47" s="8"/>
@@ -2422,12 +2510,12 @@
       <c r="Z47" s="8"/>
     </row>
     <row r="48" spans="1:26" s="9" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A48" s="23"/>
-      <c r="B48" s="27"/>
-      <c r="C48" s="34"/>
-      <c r="D48" s="24"/>
-      <c r="E48" s="36"/>
-      <c r="F48" s="21"/>
+      <c r="A48" s="39"/>
+      <c r="B48" s="38"/>
+      <c r="C48" s="41"/>
+      <c r="D48" s="40"/>
+      <c r="E48" s="43"/>
+      <c r="F48" s="49"/>
       <c r="G48" s="11"/>
       <c r="H48" s="11"/>
       <c r="I48" s="8"/>
@@ -2449,49 +2537,49 @@
       <c r="Y48" s="8"/>
       <c r="Z48" s="8"/>
     </row>
-    <row r="49" spans="1:26" s="43" customFormat="1" ht="3.75" customHeight="1">
-      <c r="A49" s="37"/>
-      <c r="B49" s="38"/>
-      <c r="C49" s="39"/>
-      <c r="D49" s="40"/>
-      <c r="E49" s="41"/>
-      <c r="F49" s="44"/>
-      <c r="G49" s="37"/>
-      <c r="H49" s="45"/>
-      <c r="I49" s="42"/>
-      <c r="J49" s="42"/>
-      <c r="K49" s="42"/>
-      <c r="L49" s="42"/>
-      <c r="M49" s="42"/>
-      <c r="N49" s="42"/>
-      <c r="O49" s="42"/>
-      <c r="P49" s="42"/>
-      <c r="Q49" s="42"/>
-      <c r="R49" s="42"/>
-      <c r="S49" s="42"/>
-      <c r="T49" s="42"/>
-      <c r="U49" s="42"/>
-      <c r="V49" s="42"/>
-      <c r="W49" s="42"/>
-      <c r="X49" s="42"/>
-      <c r="Y49" s="42"/>
-      <c r="Z49" s="42"/>
+    <row r="49" spans="1:26" s="35" customFormat="1" ht="3.75" customHeight="1">
+      <c r="A49" s="29"/>
+      <c r="B49" s="30"/>
+      <c r="C49" s="31"/>
+      <c r="D49" s="32"/>
+      <c r="E49" s="33"/>
+      <c r="F49" s="36"/>
+      <c r="G49" s="29"/>
+      <c r="H49" s="37"/>
+      <c r="I49" s="34"/>
+      <c r="J49" s="34"/>
+      <c r="K49" s="34"/>
+      <c r="L49" s="34"/>
+      <c r="M49" s="34"/>
+      <c r="N49" s="34"/>
+      <c r="O49" s="34"/>
+      <c r="P49" s="34"/>
+      <c r="Q49" s="34"/>
+      <c r="R49" s="34"/>
+      <c r="S49" s="34"/>
+      <c r="T49" s="34"/>
+      <c r="U49" s="34"/>
+      <c r="V49" s="34"/>
+      <c r="W49" s="34"/>
+      <c r="X49" s="34"/>
+      <c r="Y49" s="34"/>
+      <c r="Z49" s="34"/>
     </row>
     <row r="50" spans="1:26" s="9" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A50" s="23">
+      <c r="A50" s="39">
         <v>5</v>
       </c>
-      <c r="B50" s="27" t="s">
+      <c r="B50" s="38" t="s">
         <v>36</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>27</v>
       </c>
       <c r="E50" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="F50" s="21" t="s">
-        <v>72</v>
+        <v>91</v>
+      </c>
+      <c r="F50" s="50" t="s">
+        <v>98</v>
       </c>
       <c r="G50" s="18"/>
       <c r="H50" s="11"/>
@@ -2515,13 +2603,13 @@
       <c r="Z50" s="8"/>
     </row>
     <row r="51" spans="1:26" s="9" customFormat="1" ht="21" customHeight="1">
-      <c r="A51" s="23"/>
-      <c r="B51" s="27"/>
+      <c r="A51" s="39"/>
+      <c r="B51" s="38"/>
       <c r="C51" s="3" t="s">
         <v>28</v>
       </c>
       <c r="E51" s="10"/>
-      <c r="F51" s="21"/>
+      <c r="F51" s="48"/>
       <c r="G51" s="18"/>
       <c r="H51" s="11"/>
       <c r="I51" s="8"/>
@@ -2544,13 +2632,13 @@
       <c r="Z51" s="8"/>
     </row>
     <row r="52" spans="1:26" s="9" customFormat="1" ht="21" customHeight="1">
-      <c r="A52" s="23"/>
-      <c r="B52" s="27"/>
+      <c r="A52" s="39"/>
+      <c r="B52" s="38"/>
       <c r="C52" s="3" t="s">
         <v>29</v>
       </c>
       <c r="E52" s="10"/>
-      <c r="F52" s="21"/>
+      <c r="F52" s="49"/>
       <c r="G52" s="18"/>
       <c r="H52" s="11"/>
       <c r="I52" s="8"/>
@@ -2572,50 +2660,50 @@
       <c r="Y52" s="8"/>
       <c r="Z52" s="8"/>
     </row>
-    <row r="53" spans="1:26" s="43" customFormat="1" ht="3.75" customHeight="1">
-      <c r="A53" s="37"/>
-      <c r="B53" s="38"/>
-      <c r="C53" s="39"/>
-      <c r="D53" s="40"/>
-      <c r="E53" s="41"/>
-      <c r="F53" s="44"/>
-      <c r="G53" s="37"/>
-      <c r="H53" s="45"/>
-      <c r="I53" s="42"/>
-      <c r="J53" s="42"/>
-      <c r="K53" s="42"/>
-      <c r="L53" s="42"/>
-      <c r="M53" s="42"/>
-      <c r="N53" s="42"/>
-      <c r="O53" s="42"/>
-      <c r="P53" s="42"/>
-      <c r="Q53" s="42"/>
-      <c r="R53" s="42"/>
-      <c r="S53" s="42"/>
-      <c r="T53" s="42"/>
-      <c r="U53" s="42"/>
-      <c r="V53" s="42"/>
-      <c r="W53" s="42"/>
-      <c r="X53" s="42"/>
-      <c r="Y53" s="42"/>
-      <c r="Z53" s="42"/>
+    <row r="53" spans="1:26" s="35" customFormat="1" ht="3.75" customHeight="1">
+      <c r="A53" s="29"/>
+      <c r="B53" s="30"/>
+      <c r="C53" s="31"/>
+      <c r="D53" s="32"/>
+      <c r="E53" s="33"/>
+      <c r="F53" s="36"/>
+      <c r="G53" s="29"/>
+      <c r="H53" s="37"/>
+      <c r="I53" s="34"/>
+      <c r="J53" s="34"/>
+      <c r="K53" s="34"/>
+      <c r="L53" s="34"/>
+      <c r="M53" s="34"/>
+      <c r="N53" s="34"/>
+      <c r="O53" s="34"/>
+      <c r="P53" s="34"/>
+      <c r="Q53" s="34"/>
+      <c r="R53" s="34"/>
+      <c r="S53" s="34"/>
+      <c r="T53" s="34"/>
+      <c r="U53" s="34"/>
+      <c r="V53" s="34"/>
+      <c r="W53" s="34"/>
+      <c r="X53" s="34"/>
+      <c r="Y53" s="34"/>
+      <c r="Z53" s="34"/>
     </row>
     <row r="54" spans="1:26" s="9" customFormat="1" ht="21" customHeight="1">
-      <c r="A54" s="23">
+      <c r="A54" s="39">
         <v>6</v>
       </c>
-      <c r="B54" s="27" t="s">
+      <c r="B54" s="38" t="s">
         <v>37</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D54" s="24"/>
+      <c r="D54" s="40"/>
       <c r="E54" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="F54" s="21" t="s">
-        <v>71</v>
+      <c r="F54" s="50" t="s">
+        <v>99</v>
       </c>
       <c r="G54" s="18"/>
       <c r="H54" s="11"/>
@@ -2639,14 +2727,14 @@
       <c r="Z54" s="8"/>
     </row>
     <row r="55" spans="1:26" s="9" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A55" s="23"/>
-      <c r="B55" s="27"/>
-      <c r="C55" s="34"/>
-      <c r="D55" s="24"/>
+      <c r="A55" s="39"/>
+      <c r="B55" s="38"/>
+      <c r="C55" s="41"/>
+      <c r="D55" s="40"/>
       <c r="E55" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="F55" s="21"/>
+      <c r="F55" s="48"/>
       <c r="G55" s="18"/>
       <c r="H55" s="11"/>
       <c r="I55" s="8"/>
@@ -2669,14 +2757,14 @@
       <c r="Z55" s="8"/>
     </row>
     <row r="56" spans="1:26" s="9" customFormat="1" ht="21" customHeight="1">
-      <c r="A56" s="23"/>
-      <c r="B56" s="27"/>
-      <c r="C56" s="34"/>
-      <c r="D56" s="24"/>
+      <c r="A56" s="39"/>
+      <c r="B56" s="38"/>
+      <c r="C56" s="41"/>
+      <c r="D56" s="40"/>
       <c r="E56" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="F56" s="21"/>
+      <c r="F56" s="49"/>
       <c r="G56" s="18"/>
       <c r="H56" s="11"/>
       <c r="I56" s="8"/>
@@ -2698,33 +2786,33 @@
       <c r="Y56" s="8"/>
       <c r="Z56" s="8"/>
     </row>
-    <row r="57" spans="1:26" s="43" customFormat="1" ht="3.75" customHeight="1">
-      <c r="A57" s="37"/>
-      <c r="B57" s="38"/>
-      <c r="C57" s="39"/>
-      <c r="D57" s="40"/>
-      <c r="E57" s="41"/>
-      <c r="F57" s="44"/>
-      <c r="G57" s="37"/>
-      <c r="H57" s="45"/>
-      <c r="I57" s="42"/>
-      <c r="J57" s="42"/>
-      <c r="K57" s="42"/>
-      <c r="L57" s="42"/>
-      <c r="M57" s="42"/>
-      <c r="N57" s="42"/>
-      <c r="O57" s="42"/>
-      <c r="P57" s="42"/>
-      <c r="Q57" s="42"/>
-      <c r="R57" s="42"/>
-      <c r="S57" s="42"/>
-      <c r="T57" s="42"/>
-      <c r="U57" s="42"/>
-      <c r="V57" s="42"/>
-      <c r="W57" s="42"/>
-      <c r="X57" s="42"/>
-      <c r="Y57" s="42"/>
-      <c r="Z57" s="42"/>
+    <row r="57" spans="1:26" s="35" customFormat="1" ht="3.75" customHeight="1">
+      <c r="A57" s="29"/>
+      <c r="B57" s="30"/>
+      <c r="C57" s="31"/>
+      <c r="D57" s="32"/>
+      <c r="E57" s="33"/>
+      <c r="F57" s="36"/>
+      <c r="G57" s="29"/>
+      <c r="H57" s="37"/>
+      <c r="I57" s="34"/>
+      <c r="J57" s="34"/>
+      <c r="K57" s="34"/>
+      <c r="L57" s="34"/>
+      <c r="M57" s="34"/>
+      <c r="N57" s="34"/>
+      <c r="O57" s="34"/>
+      <c r="P57" s="34"/>
+      <c r="Q57" s="34"/>
+      <c r="R57" s="34"/>
+      <c r="S57" s="34"/>
+      <c r="T57" s="34"/>
+      <c r="U57" s="34"/>
+      <c r="V57" s="34"/>
+      <c r="W57" s="34"/>
+      <c r="X57" s="34"/>
+      <c r="Y57" s="34"/>
+      <c r="Z57" s="34"/>
     </row>
     <row r="58" spans="1:26" s="9" customFormat="1" ht="33" customHeight="1">
       <c r="A58" s="18">
@@ -2738,8 +2826,8 @@
       <c r="E58" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="F58" s="21" t="s">
-        <v>70</v>
+      <c r="F58" s="51" t="s">
+        <v>100</v>
       </c>
       <c r="G58" s="18"/>
       <c r="H58" s="11"/>
@@ -2762,39 +2850,39 @@
       <c r="Y58" s="8"/>
       <c r="Z58" s="8"/>
     </row>
-    <row r="59" spans="1:26" s="43" customFormat="1" ht="3.75" customHeight="1">
-      <c r="A59" s="37"/>
-      <c r="B59" s="38"/>
-      <c r="C59" s="39"/>
-      <c r="D59" s="40"/>
-      <c r="E59" s="41"/>
-      <c r="F59" s="44"/>
-      <c r="G59" s="37"/>
-      <c r="H59" s="45"/>
-      <c r="I59" s="42"/>
-      <c r="J59" s="42"/>
-      <c r="K59" s="42"/>
-      <c r="L59" s="42"/>
-      <c r="M59" s="42"/>
-      <c r="N59" s="42"/>
-      <c r="O59" s="42"/>
-      <c r="P59" s="42"/>
-      <c r="Q59" s="42"/>
-      <c r="R59" s="42"/>
-      <c r="S59" s="42"/>
-      <c r="T59" s="42"/>
-      <c r="U59" s="42"/>
-      <c r="V59" s="42"/>
-      <c r="W59" s="42"/>
-      <c r="X59" s="42"/>
-      <c r="Y59" s="42"/>
-      <c r="Z59" s="42"/>
+    <row r="59" spans="1:26" s="35" customFormat="1" ht="3.75" customHeight="1">
+      <c r="A59" s="29"/>
+      <c r="B59" s="30"/>
+      <c r="C59" s="31"/>
+      <c r="D59" s="32"/>
+      <c r="E59" s="33"/>
+      <c r="F59" s="36"/>
+      <c r="G59" s="29"/>
+      <c r="H59" s="37"/>
+      <c r="I59" s="34"/>
+      <c r="J59" s="34"/>
+      <c r="K59" s="34"/>
+      <c r="L59" s="34"/>
+      <c r="M59" s="34"/>
+      <c r="N59" s="34"/>
+      <c r="O59" s="34"/>
+      <c r="P59" s="34"/>
+      <c r="Q59" s="34"/>
+      <c r="R59" s="34"/>
+      <c r="S59" s="34"/>
+      <c r="T59" s="34"/>
+      <c r="U59" s="34"/>
+      <c r="V59" s="34"/>
+      <c r="W59" s="34"/>
+      <c r="X59" s="34"/>
+      <c r="Y59" s="34"/>
+      <c r="Z59" s="34"/>
     </row>
     <row r="60" spans="1:26" s="9" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A60" s="18">
+      <c r="A60" s="52">
         <v>8</v>
       </c>
-      <c r="B60" s="17" t="s">
+      <c r="B60" s="55" t="s">
         <v>39</v>
       </c>
       <c r="C60" s="3" t="s">
@@ -2804,7 +2892,9 @@
       <c r="E60" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="F60" s="21"/>
+      <c r="F60" s="50" t="s">
+        <v>102</v>
+      </c>
       <c r="G60" s="18"/>
       <c r="H60" s="11"/>
       <c r="I60" s="8"/>
@@ -2827,14 +2917,14 @@
       <c r="Z60" s="8"/>
     </row>
     <row r="61" spans="1:26" s="9" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A61" s="18"/>
-      <c r="B61" s="17"/>
+      <c r="A61" s="53"/>
+      <c r="B61" s="56"/>
       <c r="C61" s="3"/>
       <c r="D61" s="19"/>
       <c r="E61" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="F61" s="21"/>
+        <v>92</v>
+      </c>
+      <c r="F61" s="48"/>
       <c r="G61" s="18"/>
       <c r="H61" s="11"/>
       <c r="I61" s="8"/>
@@ -2857,14 +2947,14 @@
       <c r="Z61" s="8"/>
     </row>
     <row r="62" spans="1:26" s="9" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A62" s="18"/>
-      <c r="B62" s="17"/>
+      <c r="A62" s="53"/>
+      <c r="B62" s="56"/>
       <c r="C62" s="3"/>
       <c r="D62" s="19"/>
       <c r="E62" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="F62" s="21"/>
+        <v>93</v>
+      </c>
+      <c r="F62" s="48"/>
       <c r="G62" s="18"/>
       <c r="H62" s="11"/>
       <c r="I62" s="8"/>
@@ -2887,14 +2977,14 @@
       <c r="Z62" s="8"/>
     </row>
     <row r="63" spans="1:26" s="9" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A63" s="18"/>
-      <c r="B63" s="17"/>
+      <c r="A63" s="54"/>
+      <c r="B63" s="57"/>
       <c r="C63" s="3"/>
       <c r="D63" s="19"/>
       <c r="E63" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="F63" s="21"/>
+        <v>94</v>
+      </c>
+      <c r="F63" s="49"/>
       <c r="G63" s="18"/>
       <c r="H63" s="11"/>
       <c r="I63" s="8"/>
@@ -2916,33 +3006,33 @@
       <c r="Y63" s="8"/>
       <c r="Z63" s="8"/>
     </row>
-    <row r="64" spans="1:26" s="43" customFormat="1" ht="3.75" customHeight="1">
-      <c r="A64" s="37"/>
-      <c r="B64" s="38"/>
-      <c r="C64" s="39"/>
-      <c r="D64" s="40"/>
-      <c r="E64" s="41"/>
-      <c r="F64" s="44"/>
-      <c r="G64" s="37"/>
-      <c r="H64" s="45"/>
-      <c r="I64" s="42"/>
-      <c r="J64" s="42"/>
-      <c r="K64" s="42"/>
-      <c r="L64" s="42"/>
-      <c r="M64" s="42"/>
-      <c r="N64" s="42"/>
-      <c r="O64" s="42"/>
-      <c r="P64" s="42"/>
-      <c r="Q64" s="42"/>
-      <c r="R64" s="42"/>
-      <c r="S64" s="42"/>
-      <c r="T64" s="42"/>
-      <c r="U64" s="42"/>
-      <c r="V64" s="42"/>
-      <c r="W64" s="42"/>
-      <c r="X64" s="42"/>
-      <c r="Y64" s="42"/>
-      <c r="Z64" s="42"/>
+    <row r="64" spans="1:26" s="35" customFormat="1" ht="3.75" customHeight="1">
+      <c r="A64" s="29"/>
+      <c r="B64" s="30"/>
+      <c r="C64" s="31"/>
+      <c r="D64" s="32"/>
+      <c r="E64" s="33"/>
+      <c r="F64" s="36"/>
+      <c r="G64" s="29"/>
+      <c r="H64" s="37"/>
+      <c r="I64" s="34"/>
+      <c r="J64" s="34"/>
+      <c r="K64" s="34"/>
+      <c r="L64" s="34"/>
+      <c r="M64" s="34"/>
+      <c r="N64" s="34"/>
+      <c r="O64" s="34"/>
+      <c r="P64" s="34"/>
+      <c r="Q64" s="34"/>
+      <c r="R64" s="34"/>
+      <c r="S64" s="34"/>
+      <c r="T64" s="34"/>
+      <c r="U64" s="34"/>
+      <c r="V64" s="34"/>
+      <c r="W64" s="34"/>
+      <c r="X64" s="34"/>
+      <c r="Y64" s="34"/>
+      <c r="Z64" s="34"/>
     </row>
     <row r="65" spans="1:26" s="9" customFormat="1" ht="33.75" customHeight="1">
       <c r="A65" s="18">
@@ -2953,10 +3043,12 @@
       </c>
       <c r="C65" s="3"/>
       <c r="D65" s="19"/>
-      <c r="E65" s="35" t="s">
+      <c r="E65" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="F65" s="21"/>
+      <c r="F65" s="21" t="s">
+        <v>101</v>
+      </c>
       <c r="G65" s="18"/>
       <c r="H65" s="11"/>
       <c r="I65" s="8"/>
@@ -2979,17 +3071,27 @@
       <c r="Z65" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="29">
-    <mergeCell ref="B54:B56"/>
-    <mergeCell ref="A54:A56"/>
-    <mergeCell ref="D54:D56"/>
-    <mergeCell ref="A50:A52"/>
-    <mergeCell ref="B50:B52"/>
-    <mergeCell ref="C55:C56"/>
+  <mergeCells count="35">
+    <mergeCell ref="F50:F52"/>
+    <mergeCell ref="F54:F56"/>
+    <mergeCell ref="F60:F63"/>
+    <mergeCell ref="A60:A63"/>
+    <mergeCell ref="B60:B63"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B9:B27"/>
     <mergeCell ref="A9:A27"/>
     <mergeCell ref="D9:D27"/>
     <mergeCell ref="F9:F27"/>
-    <mergeCell ref="C13:C27"/>
     <mergeCell ref="A44:A48"/>
     <mergeCell ref="B44:B48"/>
     <mergeCell ref="D44:D48"/>
@@ -2997,18 +3099,14 @@
     <mergeCell ref="A37:A41"/>
     <mergeCell ref="C47:C48"/>
     <mergeCell ref="E46:E48"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B9:B27"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="F37:F42"/>
+    <mergeCell ref="F44:F48"/>
+    <mergeCell ref="B54:B56"/>
+    <mergeCell ref="A54:A56"/>
+    <mergeCell ref="D54:D56"/>
+    <mergeCell ref="A50:A52"/>
+    <mergeCell ref="B50:B52"/>
+    <mergeCell ref="C55:C56"/>
   </mergeCells>
   <conditionalFormatting sqref="B5">
     <cfRule type="cellIs" dxfId="5" priority="4" stopIfTrue="1" operator="equal">

</xml_diff>

<commit_message>
Updated RTM the with class Digram id
</commit_message>
<xml_diff>
--- a/Lhub_RTM_v1.xlsx
+++ b/Lhub_RTM_v1.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mazmy\Documents\GitHub\Learning-hub\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Farah\Desktop\V1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="112">
   <si>
     <t>Requirements Traceability Matrix</t>
   </si>
@@ -343,13 +343,79 @@
   <si>
     <t>Lhub_SDD_5.2.5
 Lhub_SDD_5.2.6</t>
+  </si>
+  <si>
+    <t>Lhub_ClassDigram_6.1.7.2.1
+Lhub_ClassDigram_6.1.7.2.2
+Lhub_ClassDigram_6.1.7.2.3
+Lhub_ClassDigram_6.1.7.2.4</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>Lhub_classDigam_6.1.2.2.3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Lhub_ClassDigram_6.1.2.2.3</t>
+  </si>
+  <si>
+    <t>Lhub_ClassDigram_6.1.2.2.4</t>
+  </si>
+  <si>
+    <t>Lhub_ClassDigram_6.1.2.2.6</t>
+  </si>
+  <si>
+    <t>Lhub_ClassDigram_6.1.3.2.1</t>
+  </si>
+  <si>
+    <t>Lhub_ClassDigram_6.1.6.2.2</t>
+  </si>
+  <si>
+    <t>Lhub_ClassDihram_6.1.5.2.6</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">          </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">  Lhub_ClassDigram_6.1.5.2.5 </t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="19">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -473,6 +539,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="1" tint="4.9989318521683403E-2"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -584,7 +657,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -689,66 +762,78 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1077,21 +1162,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="B41" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9:G36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.26953125" style="12" customWidth="1"/>
-    <col min="2" max="2" width="30.453125" style="12" customWidth="1"/>
-    <col min="3" max="3" width="48.1796875" style="12" customWidth="1"/>
-    <col min="4" max="4" width="23.26953125" style="12" customWidth="1"/>
-    <col min="5" max="5" width="35.81640625" style="12" customWidth="1"/>
+    <col min="1" max="1" width="23.28515625" style="12" customWidth="1"/>
+    <col min="2" max="2" width="30.42578125" style="12" customWidth="1"/>
+    <col min="3" max="3" width="48.140625" style="12" customWidth="1"/>
+    <col min="4" max="4" width="23.28515625" style="12" customWidth="1"/>
+    <col min="5" max="5" width="35.85546875" style="12" customWidth="1"/>
     <col min="6" max="6" width="38" style="22" customWidth="1"/>
-    <col min="7" max="7" width="37.54296875" style="12" customWidth="1"/>
-    <col min="8" max="8" width="44.54296875" style="12" customWidth="1"/>
-    <col min="9" max="16384" width="9.1796875" style="12"/>
+    <col min="7" max="7" width="37.5703125" style="12" customWidth="1"/>
+    <col min="8" max="8" width="44.5703125" style="12" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="12"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="4" customFormat="1" ht="30" customHeight="1">
@@ -1104,10 +1189,10 @@
       <c r="A2" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="44"/>
+      <c r="C2" s="53"/>
       <c r="D2" s="23" t="s">
         <v>61</v>
       </c>
@@ -1128,10 +1213,10 @@
       <c r="A3" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="44" t="s">
+      <c r="B3" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="44"/>
+      <c r="C3" s="53"/>
       <c r="D3" s="24" t="s">
         <v>66</v>
       </c>
@@ -1152,10 +1237,10 @@
       <c r="A4" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="45">
+      <c r="B4" s="54">
         <v>43470</v>
       </c>
-      <c r="C4" s="45"/>
+      <c r="C4" s="54"/>
       <c r="D4" s="25"/>
       <c r="E4" s="14">
         <v>43592</v>
@@ -1168,7 +1253,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:26" s="7" customFormat="1" ht="25">
+    <row r="5" spans="1:26" s="7" customFormat="1" ht="25.5">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -1213,22 +1298,22 @@
       <c r="Z5" s="6"/>
     </row>
     <row r="6" spans="1:26" s="9" customFormat="1" ht="24.75" customHeight="1">
-      <c r="A6" s="39">
+      <c r="A6" s="50">
         <v>1</v>
       </c>
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="55" t="s">
         <v>32</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="40"/>
+      <c r="D6" s="51"/>
       <c r="E6" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="46"/>
+      <c r="F6" s="52"/>
+      <c r="G6" s="52"/>
+      <c r="H6" s="52"/>
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
       <c r="K6" s="8"/>
@@ -1249,18 +1334,18 @@
       <c r="Z6" s="8"/>
     </row>
     <row r="7" spans="1:26" s="9" customFormat="1">
-      <c r="A7" s="39"/>
-      <c r="B7" s="38"/>
+      <c r="A7" s="50"/>
+      <c r="B7" s="55"/>
       <c r="C7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="40"/>
+      <c r="D7" s="51"/>
       <c r="E7" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="46"/>
+      <c r="F7" s="52"/>
+      <c r="G7" s="52"/>
+      <c r="H7" s="52"/>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
       <c r="K7" s="8"/>
@@ -1309,24 +1394,26 @@
       <c r="Z8" s="34"/>
     </row>
     <row r="9" spans="1:26" s="9" customFormat="1" ht="18" customHeight="1">
-      <c r="A9" s="39">
+      <c r="A9" s="50">
         <v>2</v>
       </c>
-      <c r="B9" s="38" t="s">
+      <c r="B9" s="55" t="s">
         <v>33</v>
       </c>
       <c r="C9" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="40"/>
+      <c r="D9" s="51"/>
       <c r="E9" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="F9" s="47" t="s">
+      <c r="F9" s="56" t="s">
         <v>97</v>
       </c>
-      <c r="G9" s="39"/>
-      <c r="H9" s="39"/>
+      <c r="G9" s="60" t="s">
+        <v>103</v>
+      </c>
+      <c r="H9" s="50"/>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
@@ -1347,18 +1434,18 @@
       <c r="Z9" s="8"/>
     </row>
     <row r="10" spans="1:26" s="9" customFormat="1" ht="21" customHeight="1">
-      <c r="A10" s="39"/>
-      <c r="B10" s="38"/>
+      <c r="A10" s="50"/>
+      <c r="B10" s="55"/>
       <c r="C10" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="40"/>
+      <c r="D10" s="51"/>
       <c r="E10" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="F10" s="42"/>
-      <c r="G10" s="39"/>
-      <c r="H10" s="39"/>
+      <c r="F10" s="57"/>
+      <c r="G10" s="45"/>
+      <c r="H10" s="50"/>
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
       <c r="K10" s="8"/>
@@ -1379,17 +1466,17 @@
       <c r="Z10" s="8"/>
     </row>
     <row r="11" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A11" s="39"/>
-      <c r="B11" s="38"/>
+      <c r="A11" s="50"/>
+      <c r="B11" s="55"/>
       <c r="C11" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="40"/>
+      <c r="D11" s="51"/>
       <c r="E11" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="F11" s="42"/>
-      <c r="G11" s="18"/>
+      <c r="F11" s="57"/>
+      <c r="G11" s="45"/>
       <c r="H11" s="11"/>
       <c r="I11" s="8"/>
       <c r="J11" s="8"/>
@@ -1411,17 +1498,17 @@
       <c r="Z11" s="8"/>
     </row>
     <row r="12" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A12" s="39"/>
-      <c r="B12" s="38"/>
+      <c r="A12" s="50"/>
+      <c r="B12" s="55"/>
       <c r="C12" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="D12" s="40"/>
+      <c r="D12" s="51"/>
       <c r="E12" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="F12" s="42"/>
-      <c r="G12" s="18"/>
+      <c r="F12" s="57"/>
+      <c r="G12" s="45"/>
       <c r="H12" s="11"/>
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
@@ -1443,15 +1530,15 @@
       <c r="Z12" s="8"/>
     </row>
     <row r="13" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A13" s="39"/>
-      <c r="B13" s="38"/>
-      <c r="C13" s="58"/>
-      <c r="D13" s="40"/>
+      <c r="A13" s="50"/>
+      <c r="B13" s="55"/>
+      <c r="C13" s="40"/>
+      <c r="D13" s="51"/>
       <c r="E13" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="F13" s="42"/>
-      <c r="G13" s="18"/>
+      <c r="F13" s="57"/>
+      <c r="G13" s="45"/>
       <c r="H13" s="11"/>
       <c r="I13" s="8"/>
       <c r="J13" s="8"/>
@@ -1473,15 +1560,15 @@
       <c r="Z13" s="8"/>
     </row>
     <row r="14" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A14" s="39"/>
-      <c r="B14" s="38"/>
-      <c r="C14" s="58"/>
-      <c r="D14" s="40"/>
+      <c r="A14" s="50"/>
+      <c r="B14" s="55"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="51"/>
       <c r="E14" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="F14" s="42"/>
-      <c r="G14" s="18"/>
+      <c r="F14" s="57"/>
+      <c r="G14" s="45"/>
       <c r="H14" s="11"/>
       <c r="I14" s="8"/>
       <c r="J14" s="8"/>
@@ -1503,15 +1590,15 @@
       <c r="Z14" s="8"/>
     </row>
     <row r="15" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A15" s="39"/>
-      <c r="B15" s="38"/>
-      <c r="C15" s="58"/>
-      <c r="D15" s="40"/>
+      <c r="A15" s="50"/>
+      <c r="B15" s="55"/>
+      <c r="C15" s="40"/>
+      <c r="D15" s="51"/>
       <c r="E15" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="F15" s="42"/>
-      <c r="G15" s="18"/>
+      <c r="F15" s="57"/>
+      <c r="G15" s="45"/>
       <c r="H15" s="11"/>
       <c r="I15" s="8"/>
       <c r="J15" s="8"/>
@@ -1533,15 +1620,15 @@
       <c r="Z15" s="8"/>
     </row>
     <row r="16" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A16" s="39"/>
-      <c r="B16" s="38"/>
-      <c r="C16" s="58"/>
-      <c r="D16" s="40"/>
+      <c r="A16" s="50"/>
+      <c r="B16" s="55"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="51"/>
       <c r="E16" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="F16" s="42"/>
-      <c r="G16" s="18"/>
+      <c r="F16" s="57"/>
+      <c r="G16" s="45"/>
       <c r="H16" s="11"/>
       <c r="I16" s="8"/>
       <c r="J16" s="8"/>
@@ -1563,15 +1650,15 @@
       <c r="Z16" s="8"/>
     </row>
     <row r="17" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A17" s="39"/>
-      <c r="B17" s="38"/>
-      <c r="C17" s="58"/>
-      <c r="D17" s="40"/>
+      <c r="A17" s="50"/>
+      <c r="B17" s="55"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="51"/>
       <c r="E17" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="F17" s="42"/>
-      <c r="G17" s="18"/>
+      <c r="F17" s="57"/>
+      <c r="G17" s="45"/>
       <c r="H17" s="11"/>
       <c r="I17" s="8"/>
       <c r="J17" s="8"/>
@@ -1593,15 +1680,15 @@
       <c r="Z17" s="8"/>
     </row>
     <row r="18" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A18" s="39"/>
-      <c r="B18" s="38"/>
-      <c r="C18" s="58"/>
-      <c r="D18" s="40"/>
+      <c r="A18" s="50"/>
+      <c r="B18" s="55"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="51"/>
       <c r="E18" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="F18" s="42"/>
-      <c r="G18" s="18"/>
+      <c r="F18" s="57"/>
+      <c r="G18" s="45"/>
       <c r="H18" s="11"/>
       <c r="I18" s="8"/>
       <c r="J18" s="8"/>
@@ -1623,15 +1710,15 @@
       <c r="Z18" s="8"/>
     </row>
     <row r="19" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A19" s="39"/>
-      <c r="B19" s="38"/>
-      <c r="C19" s="58"/>
-      <c r="D19" s="40"/>
+      <c r="A19" s="50"/>
+      <c r="B19" s="55"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="51"/>
       <c r="E19" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="F19" s="42"/>
-      <c r="G19" s="18"/>
+      <c r="F19" s="57"/>
+      <c r="G19" s="45"/>
       <c r="H19" s="11"/>
       <c r="I19" s="8"/>
       <c r="J19" s="8"/>
@@ -1653,15 +1740,15 @@
       <c r="Z19" s="8"/>
     </row>
     <row r="20" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A20" s="39"/>
-      <c r="B20" s="38"/>
-      <c r="C20" s="58"/>
-      <c r="D20" s="40"/>
+      <c r="A20" s="50"/>
+      <c r="B20" s="55"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="51"/>
       <c r="E20" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="F20" s="42"/>
-      <c r="G20" s="18"/>
+      <c r="F20" s="57"/>
+      <c r="G20" s="45"/>
       <c r="H20" s="11"/>
       <c r="I20" s="8"/>
       <c r="J20" s="8"/>
@@ -1683,15 +1770,15 @@
       <c r="Z20" s="8"/>
     </row>
     <row r="21" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A21" s="39"/>
-      <c r="B21" s="38"/>
-      <c r="C21" s="58"/>
-      <c r="D21" s="40"/>
+      <c r="A21" s="50"/>
+      <c r="B21" s="55"/>
+      <c r="C21" s="40"/>
+      <c r="D21" s="51"/>
       <c r="E21" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="F21" s="42"/>
-      <c r="G21" s="18"/>
+      <c r="F21" s="57"/>
+      <c r="G21" s="45"/>
       <c r="H21" s="11"/>
       <c r="I21" s="8"/>
       <c r="J21" s="8"/>
@@ -1713,15 +1800,15 @@
       <c r="Z21" s="8"/>
     </row>
     <row r="22" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A22" s="39"/>
-      <c r="B22" s="38"/>
-      <c r="C22" s="58"/>
-      <c r="D22" s="40"/>
+      <c r="A22" s="50"/>
+      <c r="B22" s="55"/>
+      <c r="C22" s="40"/>
+      <c r="D22" s="51"/>
       <c r="E22" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="F22" s="42"/>
-      <c r="G22" s="18"/>
+      <c r="F22" s="57"/>
+      <c r="G22" s="45"/>
       <c r="H22" s="11"/>
       <c r="I22" s="8"/>
       <c r="J22" s="8"/>
@@ -1743,15 +1830,15 @@
       <c r="Z22" s="8"/>
     </row>
     <row r="23" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A23" s="39"/>
-      <c r="B23" s="38"/>
-      <c r="C23" s="58"/>
-      <c r="D23" s="40"/>
+      <c r="A23" s="50"/>
+      <c r="B23" s="55"/>
+      <c r="C23" s="40"/>
+      <c r="D23" s="51"/>
       <c r="E23" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="F23" s="42"/>
-      <c r="G23" s="18"/>
+      <c r="F23" s="57"/>
+      <c r="G23" s="45"/>
       <c r="H23" s="11"/>
       <c r="I23" s="8"/>
       <c r="J23" s="8"/>
@@ -1773,15 +1860,15 @@
       <c r="Z23" s="8"/>
     </row>
     <row r="24" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A24" s="39"/>
-      <c r="B24" s="38"/>
-      <c r="C24" s="58"/>
-      <c r="D24" s="40"/>
+      <c r="A24" s="50"/>
+      <c r="B24" s="55"/>
+      <c r="C24" s="40"/>
+      <c r="D24" s="51"/>
       <c r="E24" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="F24" s="42"/>
-      <c r="G24" s="18"/>
+      <c r="F24" s="57"/>
+      <c r="G24" s="45"/>
       <c r="H24" s="11"/>
       <c r="I24" s="8"/>
       <c r="J24" s="8"/>
@@ -1803,15 +1890,15 @@
       <c r="Z24" s="8"/>
     </row>
     <row r="25" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A25" s="39"/>
-      <c r="B25" s="38"/>
-      <c r="C25" s="58"/>
-      <c r="D25" s="40"/>
+      <c r="A25" s="50"/>
+      <c r="B25" s="55"/>
+      <c r="C25" s="40"/>
+      <c r="D25" s="51"/>
       <c r="E25" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="F25" s="42"/>
-      <c r="G25" s="18"/>
+      <c r="F25" s="57"/>
+      <c r="G25" s="45"/>
       <c r="H25" s="11"/>
       <c r="I25" s="8"/>
       <c r="J25" s="8"/>
@@ -1833,15 +1920,15 @@
       <c r="Z25" s="8"/>
     </row>
     <row r="26" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A26" s="39"/>
-      <c r="B26" s="38"/>
-      <c r="C26" s="58"/>
-      <c r="D26" s="40"/>
+      <c r="A26" s="50"/>
+      <c r="B26" s="55"/>
+      <c r="C26" s="40"/>
+      <c r="D26" s="51"/>
       <c r="E26" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="F26" s="42"/>
-      <c r="G26" s="18"/>
+      <c r="F26" s="57"/>
+      <c r="G26" s="45"/>
       <c r="H26" s="11"/>
       <c r="I26" s="8"/>
       <c r="J26" s="8"/>
@@ -1863,15 +1950,15 @@
       <c r="Z26" s="8"/>
     </row>
     <row r="27" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A27" s="39"/>
-      <c r="B27" s="38"/>
-      <c r="C27" s="58"/>
-      <c r="D27" s="40"/>
+      <c r="A27" s="50"/>
+      <c r="B27" s="55"/>
+      <c r="C27" s="40"/>
+      <c r="D27" s="51"/>
       <c r="E27" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="F27" s="42"/>
-      <c r="G27" s="18"/>
+      <c r="F27" s="57"/>
+      <c r="G27" s="45"/>
       <c r="H27" s="11"/>
       <c r="I27" s="8"/>
       <c r="J27" s="8"/>
@@ -1901,7 +1988,7 @@
         <v>81</v>
       </c>
       <c r="F28" s="21"/>
-      <c r="G28" s="18"/>
+      <c r="G28" s="45"/>
       <c r="H28" s="11"/>
       <c r="I28" s="8"/>
       <c r="J28" s="8"/>
@@ -1931,7 +2018,7 @@
         <v>82</v>
       </c>
       <c r="F29" s="21"/>
-      <c r="G29" s="18"/>
+      <c r="G29" s="45"/>
       <c r="H29" s="11"/>
       <c r="I29" s="8"/>
       <c r="J29" s="8"/>
@@ -1961,7 +2048,7 @@
         <v>83</v>
       </c>
       <c r="F30" s="21"/>
-      <c r="G30" s="18"/>
+      <c r="G30" s="45"/>
       <c r="H30" s="11"/>
       <c r="I30" s="8"/>
       <c r="J30" s="8"/>
@@ -1991,7 +2078,7 @@
         <v>84</v>
       </c>
       <c r="F31" s="21"/>
-      <c r="G31" s="18"/>
+      <c r="G31" s="45"/>
       <c r="H31" s="11"/>
       <c r="I31" s="8"/>
       <c r="J31" s="8"/>
@@ -2021,7 +2108,7 @@
         <v>85</v>
       </c>
       <c r="F32" s="21"/>
-      <c r="G32" s="18"/>
+      <c r="G32" s="45"/>
       <c r="H32" s="11"/>
       <c r="I32" s="8"/>
       <c r="J32" s="8"/>
@@ -2051,7 +2138,7 @@
         <v>86</v>
       </c>
       <c r="F33" s="21"/>
-      <c r="G33" s="18"/>
+      <c r="G33" s="45"/>
       <c r="H33" s="11"/>
       <c r="I33" s="8"/>
       <c r="J33" s="8"/>
@@ -2081,7 +2168,7 @@
         <v>87</v>
       </c>
       <c r="F34" s="21"/>
-      <c r="G34" s="18"/>
+      <c r="G34" s="45"/>
       <c r="H34" s="11"/>
       <c r="I34" s="8"/>
       <c r="J34" s="8"/>
@@ -2111,7 +2198,7 @@
         <v>88</v>
       </c>
       <c r="F35" s="21"/>
-      <c r="G35" s="18"/>
+      <c r="G35" s="45"/>
       <c r="H35" s="11"/>
       <c r="I35" s="8"/>
       <c r="J35" s="8"/>
@@ -2139,7 +2226,7 @@
       <c r="D36" s="32"/>
       <c r="E36" s="33"/>
       <c r="F36" s="36"/>
-      <c r="G36" s="29"/>
+      <c r="G36" s="46"/>
       <c r="H36" s="37"/>
       <c r="I36" s="34"/>
       <c r="J36" s="34"/>
@@ -2161,10 +2248,10 @@
       <c r="Z36" s="34"/>
     </row>
     <row r="37" spans="1:26" s="9" customFormat="1" ht="27" customHeight="1">
-      <c r="A37" s="39">
+      <c r="A37" s="50">
         <v>3</v>
       </c>
-      <c r="B37" s="38" t="s">
+      <c r="B37" s="55" t="s">
         <v>34</v>
       </c>
       <c r="C37" s="3" t="s">
@@ -2173,7 +2260,7 @@
       <c r="E37" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="F37" s="50" t="s">
+      <c r="F37" s="41" t="s">
         <v>98</v>
       </c>
       <c r="G37" s="18"/>
@@ -2198,15 +2285,15 @@
       <c r="Z37" s="8"/>
     </row>
     <row r="38" spans="1:26" s="9" customFormat="1" ht="27" customHeight="1">
-      <c r="A38" s="39"/>
-      <c r="B38" s="38"/>
+      <c r="A38" s="50"/>
+      <c r="B38" s="55"/>
       <c r="C38" s="3" t="s">
         <v>20</v>
       </c>
       <c r="E38" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="F38" s="48"/>
+      <c r="F38" s="42"/>
       <c r="G38" s="18"/>
       <c r="H38" s="11"/>
       <c r="I38" s="8"/>
@@ -2229,15 +2316,15 @@
       <c r="Z38" s="8"/>
     </row>
     <row r="39" spans="1:26" s="9" customFormat="1" ht="27" customHeight="1">
-      <c r="A39" s="39"/>
-      <c r="B39" s="38"/>
+      <c r="A39" s="50"/>
+      <c r="B39" s="55"/>
       <c r="C39" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E39" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="F39" s="48"/>
+      <c r="F39" s="42"/>
       <c r="G39" s="18"/>
       <c r="H39" s="11"/>
       <c r="I39" s="8"/>
@@ -2260,8 +2347,8 @@
       <c r="Z39" s="8"/>
     </row>
     <row r="40" spans="1:26" s="9" customFormat="1" ht="27" customHeight="1">
-      <c r="A40" s="39"/>
-      <c r="B40" s="38"/>
+      <c r="A40" s="50"/>
+      <c r="B40" s="55"/>
       <c r="C40" s="3" t="s">
         <v>22</v>
       </c>
@@ -2269,7 +2356,7 @@
       <c r="E40" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="F40" s="48"/>
+      <c r="F40" s="42"/>
       <c r="G40" s="18"/>
       <c r="H40" s="11"/>
       <c r="I40" s="8"/>
@@ -2292,8 +2379,8 @@
       <c r="Z40" s="8"/>
     </row>
     <row r="41" spans="1:26" s="9" customFormat="1" ht="27" customHeight="1">
-      <c r="A41" s="39"/>
-      <c r="B41" s="38"/>
+      <c r="A41" s="50"/>
+      <c r="B41" s="55"/>
       <c r="C41" s="3" t="s">
         <v>23</v>
       </c>
@@ -2301,7 +2388,7 @@
       <c r="E41" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="F41" s="48"/>
+      <c r="F41" s="42"/>
       <c r="G41" s="18"/>
       <c r="H41" s="11"/>
       <c r="I41" s="8"/>
@@ -2331,8 +2418,10 @@
       <c r="E42" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="F42" s="49"/>
-      <c r="G42" s="18"/>
+      <c r="F42" s="43"/>
+      <c r="G42" s="18" t="s">
+        <v>104</v>
+      </c>
       <c r="H42" s="11"/>
       <c r="I42" s="8"/>
       <c r="J42" s="8"/>
@@ -2382,23 +2471,25 @@
       <c r="Z43" s="34"/>
     </row>
     <row r="44" spans="1:26" s="9" customFormat="1" ht="21.75" customHeight="1">
-      <c r="A44" s="39">
+      <c r="A44" s="50">
         <v>4</v>
       </c>
-      <c r="B44" s="38" t="s">
+      <c r="B44" s="55" t="s">
         <v>35</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D44" s="40"/>
+      <c r="D44" s="51"/>
       <c r="E44" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="F44" s="50" t="s">
+      <c r="F44" s="41" t="s">
         <v>98</v>
       </c>
-      <c r="G44" s="11"/>
+      <c r="G44" s="62" t="s">
+        <v>111</v>
+      </c>
       <c r="H44" s="11"/>
       <c r="I44" s="8"/>
       <c r="J44" s="8"/>
@@ -2420,16 +2511,16 @@
       <c r="Z44" s="8"/>
     </row>
     <row r="45" spans="1:26" s="9" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A45" s="39"/>
-      <c r="B45" s="38"/>
+      <c r="A45" s="50"/>
+      <c r="B45" s="55"/>
       <c r="C45" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D45" s="40"/>
+      <c r="D45" s="51"/>
       <c r="E45" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="F45" s="48"/>
+      <c r="F45" s="42"/>
       <c r="G45" s="11"/>
       <c r="H45" s="11"/>
       <c r="I45" s="8"/>
@@ -2452,14 +2543,14 @@
       <c r="Z45" s="8"/>
     </row>
     <row r="46" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A46" s="39"/>
-      <c r="B46" s="38"/>
+      <c r="A46" s="50"/>
+      <c r="B46" s="55"/>
       <c r="C46" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D46" s="40"/>
-      <c r="E46" s="43"/>
-      <c r="F46" s="48"/>
+      <c r="D46" s="51"/>
+      <c r="E46" s="59"/>
+      <c r="F46" s="42"/>
       <c r="G46" s="11"/>
       <c r="H46" s="11"/>
       <c r="I46" s="8"/>
@@ -2482,12 +2573,12 @@
       <c r="Z46" s="8"/>
     </row>
     <row r="47" spans="1:26" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A47" s="39"/>
-      <c r="B47" s="38"/>
-      <c r="C47" s="41"/>
-      <c r="D47" s="40"/>
-      <c r="E47" s="43"/>
-      <c r="F47" s="48"/>
+      <c r="A47" s="50"/>
+      <c r="B47" s="55"/>
+      <c r="C47" s="58"/>
+      <c r="D47" s="51"/>
+      <c r="E47" s="59"/>
+      <c r="F47" s="42"/>
       <c r="G47" s="11"/>
       <c r="H47" s="11"/>
       <c r="I47" s="8"/>
@@ -2510,12 +2601,12 @@
       <c r="Z47" s="8"/>
     </row>
     <row r="48" spans="1:26" s="9" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A48" s="39"/>
-      <c r="B48" s="38"/>
-      <c r="C48" s="41"/>
-      <c r="D48" s="40"/>
-      <c r="E48" s="43"/>
-      <c r="F48" s="49"/>
+      <c r="A48" s="50"/>
+      <c r="B48" s="55"/>
+      <c r="C48" s="58"/>
+      <c r="D48" s="51"/>
+      <c r="E48" s="59"/>
+      <c r="F48" s="43"/>
       <c r="G48" s="11"/>
       <c r="H48" s="11"/>
       <c r="I48" s="8"/>
@@ -2566,10 +2657,10 @@
       <c r="Z49" s="34"/>
     </row>
     <row r="50" spans="1:26" s="9" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A50" s="39">
+      <c r="A50" s="50">
         <v>5</v>
       </c>
-      <c r="B50" s="38" t="s">
+      <c r="B50" s="55" t="s">
         <v>36</v>
       </c>
       <c r="C50" s="3" t="s">
@@ -2578,7 +2669,7 @@
       <c r="E50" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="F50" s="50" t="s">
+      <c r="F50" s="41" t="s">
         <v>98</v>
       </c>
       <c r="G50" s="18"/>
@@ -2603,14 +2694,16 @@
       <c r="Z50" s="8"/>
     </row>
     <row r="51" spans="1:26" s="9" customFormat="1" ht="21" customHeight="1">
-      <c r="A51" s="39"/>
-      <c r="B51" s="38"/>
+      <c r="A51" s="50"/>
+      <c r="B51" s="55"/>
       <c r="C51" s="3" t="s">
         <v>28</v>
       </c>
       <c r="E51" s="10"/>
-      <c r="F51" s="48"/>
-      <c r="G51" s="18"/>
+      <c r="F51" s="42"/>
+      <c r="G51" s="61" t="s">
+        <v>110</v>
+      </c>
       <c r="H51" s="11"/>
       <c r="I51" s="8"/>
       <c r="J51" s="8"/>
@@ -2632,13 +2725,13 @@
       <c r="Z51" s="8"/>
     </row>
     <row r="52" spans="1:26" s="9" customFormat="1" ht="21" customHeight="1">
-      <c r="A52" s="39"/>
-      <c r="B52" s="38"/>
+      <c r="A52" s="50"/>
+      <c r="B52" s="55"/>
       <c r="C52" s="3" t="s">
         <v>29</v>
       </c>
       <c r="E52" s="10"/>
-      <c r="F52" s="49"/>
+      <c r="F52" s="43"/>
       <c r="G52" s="18"/>
       <c r="H52" s="11"/>
       <c r="I52" s="8"/>
@@ -2689,23 +2782,23 @@
       <c r="Z53" s="34"/>
     </row>
     <row r="54" spans="1:26" s="9" customFormat="1" ht="21" customHeight="1">
-      <c r="A54" s="39">
+      <c r="A54" s="50">
         <v>6</v>
       </c>
-      <c r="B54" s="38" t="s">
+      <c r="B54" s="55" t="s">
         <v>37</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D54" s="40"/>
+      <c r="D54" s="51"/>
       <c r="E54" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="F54" s="50" t="s">
+      <c r="F54" s="41" t="s">
         <v>99</v>
       </c>
-      <c r="G54" s="18"/>
+      <c r="G54" s="38"/>
       <c r="H54" s="11"/>
       <c r="I54" s="8"/>
       <c r="J54" s="8"/>
@@ -2727,15 +2820,17 @@
       <c r="Z54" s="8"/>
     </row>
     <row r="55" spans="1:26" s="9" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A55" s="39"/>
-      <c r="B55" s="38"/>
-      <c r="C55" s="41"/>
-      <c r="D55" s="40"/>
+      <c r="A55" s="50"/>
+      <c r="B55" s="55"/>
+      <c r="C55" s="58"/>
+      <c r="D55" s="51"/>
       <c r="E55" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="F55" s="48"/>
-      <c r="G55" s="18"/>
+      <c r="F55" s="42"/>
+      <c r="G55" s="61" t="s">
+        <v>105</v>
+      </c>
       <c r="H55" s="11"/>
       <c r="I55" s="8"/>
       <c r="J55" s="8"/>
@@ -2757,15 +2852,17 @@
       <c r="Z55" s="8"/>
     </row>
     <row r="56" spans="1:26" s="9" customFormat="1" ht="21" customHeight="1">
-      <c r="A56" s="39"/>
-      <c r="B56" s="38"/>
-      <c r="C56" s="41"/>
-      <c r="D56" s="40"/>
+      <c r="A56" s="50"/>
+      <c r="B56" s="55"/>
+      <c r="C56" s="58"/>
+      <c r="D56" s="51"/>
       <c r="E56" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="F56" s="49"/>
-      <c r="G56" s="18"/>
+      <c r="F56" s="43"/>
+      <c r="G56" s="61" t="s">
+        <v>106</v>
+      </c>
       <c r="H56" s="11"/>
       <c r="I56" s="8"/>
       <c r="J56" s="8"/>
@@ -2826,10 +2923,12 @@
       <c r="E58" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="F58" s="51" t="s">
+      <c r="F58" s="39" t="s">
         <v>100</v>
       </c>
-      <c r="G58" s="18"/>
+      <c r="G58" s="61" t="s">
+        <v>107</v>
+      </c>
       <c r="H58" s="11"/>
       <c r="I58" s="8"/>
       <c r="J58" s="8"/>
@@ -2879,10 +2978,10 @@
       <c r="Z59" s="34"/>
     </row>
     <row r="60" spans="1:26" s="9" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A60" s="52">
+      <c r="A60" s="44">
         <v>8</v>
       </c>
-      <c r="B60" s="55" t="s">
+      <c r="B60" s="47" t="s">
         <v>39</v>
       </c>
       <c r="C60" s="3" t="s">
@@ -2892,10 +2991,12 @@
       <c r="E60" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="F60" s="50" t="s">
+      <c r="F60" s="41" t="s">
         <v>102</v>
       </c>
-      <c r="G60" s="18"/>
+      <c r="G60" s="61" t="s">
+        <v>108</v>
+      </c>
       <c r="H60" s="11"/>
       <c r="I60" s="8"/>
       <c r="J60" s="8"/>
@@ -2917,15 +3018,17 @@
       <c r="Z60" s="8"/>
     </row>
     <row r="61" spans="1:26" s="9" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A61" s="53"/>
-      <c r="B61" s="56"/>
+      <c r="A61" s="45"/>
+      <c r="B61" s="48"/>
       <c r="C61" s="3"/>
       <c r="D61" s="19"/>
       <c r="E61" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="F61" s="48"/>
-      <c r="G61" s="18"/>
+      <c r="F61" s="42"/>
+      <c r="G61" s="61" t="s">
+        <v>109</v>
+      </c>
       <c r="H61" s="11"/>
       <c r="I61" s="8"/>
       <c r="J61" s="8"/>
@@ -2947,14 +3050,14 @@
       <c r="Z61" s="8"/>
     </row>
     <row r="62" spans="1:26" s="9" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A62" s="53"/>
-      <c r="B62" s="56"/>
+      <c r="A62" s="45"/>
+      <c r="B62" s="48"/>
       <c r="C62" s="3"/>
       <c r="D62" s="19"/>
       <c r="E62" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="F62" s="48"/>
+      <c r="F62" s="42"/>
       <c r="G62" s="18"/>
       <c r="H62" s="11"/>
       <c r="I62" s="8"/>
@@ -2977,14 +3080,14 @@
       <c r="Z62" s="8"/>
     </row>
     <row r="63" spans="1:26" s="9" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A63" s="54"/>
-      <c r="B63" s="57"/>
+      <c r="A63" s="46"/>
+      <c r="B63" s="49"/>
       <c r="C63" s="3"/>
       <c r="D63" s="19"/>
       <c r="E63" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="F63" s="49"/>
+      <c r="F63" s="43"/>
       <c r="G63" s="18"/>
       <c r="H63" s="11"/>
       <c r="I63" s="8"/>
@@ -3072,23 +3175,7 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="F50:F52"/>
-    <mergeCell ref="F54:F56"/>
-    <mergeCell ref="F60:F63"/>
-    <mergeCell ref="A60:A63"/>
-    <mergeCell ref="B60:B63"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B9:B27"/>
+    <mergeCell ref="G9:G36"/>
     <mergeCell ref="A9:A27"/>
     <mergeCell ref="D9:D27"/>
     <mergeCell ref="F9:F27"/>
@@ -3101,6 +3188,22 @@
     <mergeCell ref="E46:E48"/>
     <mergeCell ref="F37:F42"/>
     <mergeCell ref="F44:F48"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B9:B27"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="F50:F52"/>
+    <mergeCell ref="F54:F56"/>
+    <mergeCell ref="F60:F63"/>
+    <mergeCell ref="A60:A63"/>
+    <mergeCell ref="B60:B63"/>
     <mergeCell ref="B54:B56"/>
     <mergeCell ref="A54:A56"/>
     <mergeCell ref="D54:D56"/>

</xml_diff>